<commit_message>
No savings data in a month
</commit_message>
<xml_diff>
--- a/2024/OAS 2024.xlsx
+++ b/2024/OAS 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnbar\Dropbox\OAS\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331BAC63-074D-4975-A306-EC879CB93DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86880FFB-0569-4D8C-BA13-69DD543AF1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="9" activeTab="10" xr2:uid="{E6A7689A-682B-425D-92A3-B87F804748A5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="7" activeTab="8" xr2:uid="{E6A7689A-682B-425D-92A3-B87F804748A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="8" r:id="rId1"/>
@@ -35,8 +35,8 @@
   <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId15"/>
-    <pivotCache cacheId="1" r:id="rId16"/>
-    <pivotCache cacheId="2" r:id="rId17"/>
+    <pivotCache cacheId="7" r:id="rId16"/>
+    <pivotCache cacheId="11" r:id="rId17"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4793" uniqueCount="2231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4813" uniqueCount="2235">
   <si>
     <t>Subs</t>
   </si>
@@ -6673,9 +6673,6 @@
     <t>Stripe fees (including fees paid on refunds)</t>
   </si>
   <si>
-    <t>aa</t>
-  </si>
-  <si>
     <t>SumUp Payments AccMDD PID724802</t>
   </si>
   <si>
@@ -6749,6 +6746,21 @@
   </si>
   <si>
     <t>SumUp Payments AccMDD PID731586</t>
+  </si>
+  <si>
+    <t>Two sales?</t>
+  </si>
+  <si>
+    <t>SumUp Payments AccMDD PID736355</t>
+  </si>
+  <si>
+    <t>Martyn Burdon OAS prize</t>
+  </si>
+  <si>
+    <t>SumUp Payments AccMDD PID737882</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prizewinner forgot to cash cheque </t>
   </si>
 </sst>
 </file>
@@ -6903,7 +6915,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -6948,6 +6960,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -7012,13 +7025,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45562.842416087966" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="316" xr:uid="{52AA0CD4-A3EB-4892-953B-4445B6BC29AB}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45567.394030324074" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="320" xr:uid="{52AA0CD4-A3EB-4892-953B-4445B6BC29AB}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I502" sheet="Current account"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2024-01-01T00:00:00" maxDate="2024-09-28T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2024-01-01T00:00:00" maxDate="2024-10-02T00:00:00"/>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -7083,13 +7096,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45562.842449999996" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="316" xr:uid="{133830F7-3A79-4A2B-AFB2-D11D3864E8D7}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45567.394124768522" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="320" xr:uid="{133830F7-3A79-4A2B-AFB2-D11D3864E8D7}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:H501" sheet="Current account"/>
   </cacheSource>
   <cacheFields count="8">
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2024-01-01T00:00:00" maxDate="2024-09-28T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2024-01-01T00:00:00" maxDate="2024-10-02T00:00:00"/>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -9051,7 +9064,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="316">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="320">
   <r>
     <d v="2024-01-01T00:00:00"/>
     <s v="CR"/>
@@ -12518,6 +12531,50 @@
     <m/>
   </r>
   <r>
+    <d v="2024-09-30T00:00:00"/>
+    <s v="CR"/>
+    <s v="Stripe Payments UKSTRIPE"/>
+    <m/>
+    <n v="344.55"/>
+    <n v="10989.799999999992"/>
+    <x v="6"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-09-30T00:00:00"/>
+    <s v="CR"/>
+    <s v="SumUp Payments AccMDD PID736355"/>
+    <m/>
+    <n v="742.24"/>
+    <n v="11732.039999999992"/>
+    <x v="6"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-01T00:00:00"/>
+    <s v="BP"/>
+    <s v="Martyn Burdon OAS prize"/>
+    <n v="100"/>
+    <m/>
+    <n v="11632.039999999992"/>
+    <x v="7"/>
+    <x v="1"/>
+    <s v="Prizewinner forgot to cash cheque "/>
+  </r>
+  <r>
+    <d v="2024-10-01T00:00:00"/>
+    <s v="CR"/>
+    <s v="SumUp Payments AccMDD PID737882"/>
+    <m/>
+    <n v="221.2"/>
+    <n v="11853.239999999993"/>
+    <x v="6"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
     <m/>
     <m/>
     <m/>
@@ -12532,7 +12589,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="316">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="320">
   <r>
     <d v="2024-01-01T00:00:00"/>
     <s v="CR"/>
@@ -15680,6 +15737,46 @@
     <m/>
     <n v="294.93"/>
     <n v="10645.249999999993"/>
+    <x v="6"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-09-30T00:00:00"/>
+    <s v="CR"/>
+    <s v="Stripe Payments UKSTRIPE"/>
+    <m/>
+    <n v="344.55"/>
+    <n v="10989.799999999992"/>
+    <x v="6"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-09-30T00:00:00"/>
+    <s v="CR"/>
+    <s v="SumUp Payments AccMDD PID736355"/>
+    <m/>
+    <n v="742.24"/>
+    <n v="11732.039999999992"/>
+    <x v="6"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-01T00:00:00"/>
+    <s v="BP"/>
+    <s v="Martyn Burdon OAS prize"/>
+    <n v="100"/>
+    <m/>
+    <n v="11632.039999999992"/>
+    <x v="7"/>
+    <s v="Members"/>
+  </r>
+  <r>
+    <d v="2024-10-01T00:00:00"/>
+    <s v="CR"/>
+    <s v="SumUp Payments AccMDD PID737882"/>
+    <m/>
+    <n v="221.2"/>
+    <n v="11853.239999999993"/>
     <x v="6"/>
     <s v="Open"/>
   </r>
@@ -15768,7 +15865,72 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BE04C0F0-9A61-4F80-8276-3D04382D746D}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A5C2633A-7AD5-4920-9B01-65373321B481}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E4:G8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField numFmtId="15" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Income" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Expenditure" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BE04C0F0-9A61-4F80-8276-3D04382D746D}" name="PivotTable2" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C28" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField numFmtId="15" showAll="0"/>
@@ -15915,181 +16077,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A5C2633A-7AD5-4920-9B01-65373321B481}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="E4:G8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField numFmtId="15" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="7"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Income" fld="4" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Expenditure" fld="3" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2FE7C9AF-75EF-4873-8F1B-0F70A39EEC38}" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A19:C27" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="9">
-    <pivotField numFmtId="15" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="25">
-        <item x="1"/>
-        <item x="14"/>
-        <item x="4"/>
-        <item x="15"/>
-        <item x="10"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="12"/>
-        <item x="9"/>
-        <item x="11"/>
-        <item x="6"/>
-        <item x="13"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="16"/>
-        <item x="23"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="8"/>
-        <item x="21"/>
-        <item x="5"/>
-        <item x="22"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="6"/>
-  </rowFields>
-  <rowItems count="8">
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="7" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Sum of Income" fld="4" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Expenditure" fld="3" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{88CC6FF2-D2D5-4EC7-9086-AAE36B3B0E13}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{88CC6FF2-D2D5-4EC7-9086-AAE36B3B0E13}" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="15" showAll="0"/>
@@ -16188,6 +16177,114 @@
   </colItems>
   <pageFields count="1">
     <pageField fld="7" item="0" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Sum of Income" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Expenditure" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2FE7C9AF-75EF-4873-8F1B-0F70A39EEC38}" name="PivotTable5" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A19:C27" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="9">
+    <pivotField numFmtId="15" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="25">
+        <item x="1"/>
+        <item x="14"/>
+        <item x="4"/>
+        <item x="15"/>
+        <item x="10"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="12"/>
+        <item x="9"/>
+        <item x="11"/>
+        <item x="6"/>
+        <item x="13"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="16"/>
+        <item x="23"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="8"/>
+        <item x="21"/>
+        <item x="5"/>
+        <item x="22"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="7" item="1" hier="-1"/>
   </pageFields>
   <dataFields count="2">
     <dataField name="Sum of Income" fld="4" baseField="0" baseItem="0"/>
@@ -16639,7 +16736,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>2218</v>
+        <v>2217</v>
       </c>
       <c r="C5" s="19">
         <f>'Members Exhibition'!C14</f>
@@ -16651,7 +16748,7 @@
       </c>
       <c r="F5" s="19">
         <f>GETPIVOTDATA("Sum of Expenditure",Exhibitions!$A$3,"Category","Prizes")</f>
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
@@ -16873,7 +16970,7 @@
       <c r="E11" s="19"/>
       <c r="F11" s="19">
         <f>SUM(F5:F10)</f>
-        <v>3925.3600000000006</v>
+        <v>4025.3600000000006</v>
       </c>
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
@@ -16883,7 +16980,7 @@
       <c r="J11" s="19"/>
       <c r="K11" s="19">
         <f>F33</f>
-        <v>1060.4399999999994</v>
+        <v>960.43999999999937</v>
       </c>
       <c r="L11" s="19"/>
       <c r="M11" s="19" t="s">
@@ -16945,7 +17042,7 @@
       </c>
       <c r="F13" s="19">
         <f>C15-F11</f>
-        <v>-617.88000000000056</v>
+        <v>-717.88000000000056</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
@@ -17024,7 +17121,7 @@
       <c r="J15" s="19"/>
       <c r="K15" s="19">
         <f>SUM(K4:K11)</f>
-        <v>1345.3299999999995</v>
+        <v>1245.3299999999995</v>
       </c>
       <c r="L15" s="19"/>
       <c r="M15" s="19"/>
@@ -17084,7 +17181,7 @@
       <c r="N17" s="19"/>
       <c r="O17" s="19">
         <f>K15-O15</f>
-        <v>1345.3299999999995</v>
+        <v>1245.3299999999995</v>
       </c>
       <c r="P17" s="28"/>
       <c r="R17" s="5" t="s">
@@ -17146,14 +17243,14 @@
       <c r="J19" s="19"/>
       <c r="K19" s="22">
         <f>K15</f>
-        <v>1345.3299999999995</v>
+        <v>1245.3299999999995</v>
       </c>
       <c r="L19" s="19"/>
       <c r="M19" s="19"/>
       <c r="N19" s="19"/>
       <c r="O19" s="22">
         <f>K19</f>
-        <v>1345.3299999999995</v>
+        <v>1245.3299999999995</v>
       </c>
       <c r="R19" s="5" t="s">
         <v>10</v>
@@ -17164,7 +17261,7 @@
       </c>
       <c r="T19" s="28">
         <f>F5+F20</f>
-        <v>500</v>
+        <v>600</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="13.5" thickTop="1" x14ac:dyDescent="0.3">
@@ -17230,15 +17327,15 @@
       </c>
       <c r="T21" s="5">
         <f>SUM(T10:T19)</f>
-        <v>2247.0400000000009</v>
+        <v>2347.0400000000009</v>
       </c>
       <c r="U21" s="28">
         <f>O15+F11+F26</f>
-        <v>2247.0400000000009</v>
+        <v>2347.0400000000009</v>
       </c>
       <c r="V21" s="28">
         <f>S21-U21</f>
-        <v>-2247.0400000000009</v>
+        <v>-2347.0400000000009</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
@@ -17307,11 +17404,11 @@
       </c>
       <c r="T23" s="13">
         <f>SUM(T4:T6)-SUM(T10:T19)</f>
-        <v>1210.4399999999991</v>
+        <v>1110.4399999999991</v>
       </c>
       <c r="U23" s="13">
         <f>S23-T23</f>
-        <v>-1210.4399999999991</v>
+        <v>-1110.4399999999991</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
@@ -17522,7 +17619,7 @@
       <c r="E33" s="19"/>
       <c r="F33" s="24">
         <f>F28+F13</f>
-        <v>1060.4399999999994</v>
+        <v>960.43999999999937</v>
       </c>
       <c r="G33" s="18"/>
       <c r="H33" s="18"/>
@@ -17572,7 +17669,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -17605,15 +17702,17 @@
       <c r="A4" s="34" t="s">
         <v>812</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="40">
         <v>100</v>
       </c>
+      <c r="C4" s="40"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>864</v>
       </c>
-      <c r="C5">
+      <c r="B5" s="40"/>
+      <c r="C5" s="40">
         <v>1500</v>
       </c>
     </row>
@@ -17621,15 +17720,17 @@
       <c r="A6" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C6">
-        <v>500</v>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40">
+        <v>600</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="C7">
+      <c r="B7" s="40"/>
+      <c r="C7" s="40">
         <v>550</v>
       </c>
     </row>
@@ -17637,7 +17738,8 @@
       <c r="A8" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C8">
+      <c r="B8" s="40"/>
+      <c r="C8" s="40">
         <v>175</v>
       </c>
     </row>
@@ -17645,15 +17747,17 @@
       <c r="A9" s="34" t="s">
         <v>808</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="40">
         <v>3623.6800000000003</v>
       </c>
+      <c r="C9" s="40"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
         <v>809</v>
       </c>
-      <c r="C10">
+      <c r="B10" s="40"/>
+      <c r="C10" s="40">
         <v>2632.5</v>
       </c>
     </row>
@@ -17661,15 +17765,17 @@
       <c r="A11" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="40">
         <v>2604.98</v>
       </c>
+      <c r="C11" s="40"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
         <v>863</v>
       </c>
-      <c r="C12">
+      <c r="B12" s="40"/>
+      <c r="C12" s="40">
         <v>1261.68</v>
       </c>
       <c r="I12">
@@ -17679,21 +17785,22 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
-        <v>2208</v>
-      </c>
-      <c r="B13">
+        <v>2207</v>
+      </c>
+      <c r="B13" s="40">
         <v>178.99</v>
       </c>
+      <c r="C13" s="40"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
         <v>573</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="40">
         <v>6507.65</v>
       </c>
-      <c r="C14">
-        <v>6619.18</v>
+      <c r="C14" s="40">
+        <v>6719.18</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -17736,7 +17843,8 @@
       <c r="A20" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C20">
+      <c r="B20" s="40"/>
+      <c r="C20" s="40">
         <v>200</v>
       </c>
       <c r="E20" t="s">
@@ -17756,7 +17864,8 @@
       <c r="A21" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="C21">
+      <c r="B21" s="40"/>
+      <c r="C21" s="40">
         <v>223</v>
       </c>
       <c r="E21" t="s">
@@ -17767,16 +17876,14 @@
       </c>
       <c r="H21">
         <v>312</v>
-      </c>
-      <c r="I21" t="s">
-        <v>2205</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C22">
+      <c r="B22" s="40"/>
+      <c r="C22" s="40">
         <v>126</v>
       </c>
       <c r="E22" t="s">
@@ -17795,42 +17902,46 @@
       <c r="A23" s="34" t="s">
         <v>808</v>
       </c>
-      <c r="B23">
-        <v>2400.2799999999997</v>
-      </c>
+      <c r="B23" s="40">
+        <v>3708.27</v>
+      </c>
+      <c r="C23" s="40"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="40">
         <v>8007.4999999999991</v>
       </c>
+      <c r="C24" s="40"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="34" t="s">
         <v>811</v>
       </c>
-      <c r="C25">
+      <c r="B25" s="40"/>
+      <c r="C25" s="40">
         <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="34" t="s">
-        <v>2208</v>
-      </c>
-      <c r="B26">
+        <v>2207</v>
+      </c>
+      <c r="B26" s="40">
         <v>116.57</v>
       </c>
+      <c r="C26" s="40"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="34" t="s">
         <v>573</v>
       </c>
-      <c r="B27">
-        <v>10524.349999999999</v>
-      </c>
-      <c r="C27">
+      <c r="B27" s="40">
+        <v>11832.339999999998</v>
+      </c>
+      <c r="C27" s="40">
         <v>780</v>
       </c>
     </row>
@@ -17841,10 +17952,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5956F534-76F9-4C2C-AE0C-5DBCF3D7B234}">
-  <dimension ref="A1:I316"/>
+  <dimension ref="A1:I320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A293" workbookViewId="0">
-      <selection activeCell="G306" sqref="G306"/>
+    <sheetView topLeftCell="A296" workbookViewId="0">
+      <selection activeCell="I319" sqref="I319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -22162,7 +22273,7 @@
         <v>7</v>
       </c>
       <c r="I203" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
@@ -22300,7 +22411,7 @@
         <v>14806.09</v>
       </c>
       <c r="G209" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="H209" t="s">
         <v>869</v>
@@ -22314,7 +22425,7 @@
         <v>396</v>
       </c>
       <c r="C210" t="s">
-        <v>2219</v>
+        <v>2218</v>
       </c>
       <c r="E210">
         <v>663.59</v>
@@ -22540,7 +22651,7 @@
         <v>16195.59</v>
       </c>
       <c r="G219" t="s">
-        <v>2213</v>
+        <v>2212</v>
       </c>
       <c r="I219" t="s">
         <v>865</v>
@@ -23499,7 +23610,7 @@
         <v>18</v>
       </c>
       <c r="F261" s="32">
-        <f t="shared" ref="F261:F316" si="4">F260+E261-D261</f>
+        <f t="shared" ref="F261:F320" si="4">F260+E261-D261</f>
         <v>8348.1099999999951</v>
       </c>
       <c r="G261" t="s">
@@ -24609,7 +24720,7 @@
         <v>396</v>
       </c>
       <c r="C308" t="s">
-        <v>2206</v>
+        <v>2205</v>
       </c>
       <c r="E308">
         <v>116.57</v>
@@ -24619,7 +24730,7 @@
         <v>15321.919999999995</v>
       </c>
       <c r="G308" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="H308" t="s">
         <v>870</v>
@@ -24630,7 +24741,7 @@
         <v>45558</v>
       </c>
       <c r="C309" t="s">
-        <v>2207</v>
+        <v>2206</v>
       </c>
       <c r="E309">
         <v>1558.21</v>
@@ -24651,10 +24762,10 @@
         <v>45560</v>
       </c>
       <c r="B310" t="s">
+        <v>2208</v>
+      </c>
+      <c r="C310" t="s">
         <v>2209</v>
-      </c>
-      <c r="C310" t="s">
-        <v>2210</v>
       </c>
       <c r="D310">
         <v>6000</v>
@@ -24675,7 +24786,7 @@
         <v>541</v>
       </c>
       <c r="C311" t="s">
-        <v>2215</v>
+        <v>2214</v>
       </c>
       <c r="D311">
         <v>18</v>
@@ -24699,7 +24810,7 @@
         <v>541</v>
       </c>
       <c r="C312" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
       <c r="D312">
         <v>118.95</v>
@@ -24720,7 +24831,7 @@
         <v>396</v>
       </c>
       <c r="C313" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
       <c r="E313">
         <v>457.14</v>
@@ -24744,7 +24855,7 @@
         <v>541</v>
       </c>
       <c r="C314" t="s">
-        <v>2220</v>
+        <v>2219</v>
       </c>
       <c r="D314">
         <v>650</v>
@@ -24781,7 +24892,7 @@
         <v>870</v>
       </c>
       <c r="I315" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
     </row>
     <row r="316" spans="1:9" x14ac:dyDescent="0.25">
@@ -24792,7 +24903,7 @@
         <v>396</v>
       </c>
       <c r="C316" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
       <c r="E316">
         <v>294.93</v>
@@ -24805,6 +24916,105 @@
         <v>808</v>
       </c>
       <c r="H316" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A317" s="31">
+        <v>45565</v>
+      </c>
+      <c r="B317" t="s">
+        <v>396</v>
+      </c>
+      <c r="C317" t="s">
+        <v>828</v>
+      </c>
+      <c r="E317">
+        <v>344.55</v>
+      </c>
+      <c r="F317" s="32">
+        <f t="shared" si="4"/>
+        <v>10989.799999999992</v>
+      </c>
+      <c r="G317" t="s">
+        <v>808</v>
+      </c>
+      <c r="H317" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="318" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A318" s="31">
+        <v>45565</v>
+      </c>
+      <c r="B318" t="s">
+        <v>396</v>
+      </c>
+      <c r="C318" t="s">
+        <v>2231</v>
+      </c>
+      <c r="E318">
+        <v>742.24</v>
+      </c>
+      <c r="F318" s="32">
+        <f t="shared" si="4"/>
+        <v>11732.039999999992</v>
+      </c>
+      <c r="G318" t="s">
+        <v>808</v>
+      </c>
+      <c r="H318" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="319" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A319" s="31">
+        <v>45566</v>
+      </c>
+      <c r="B319" t="s">
+        <v>541</v>
+      </c>
+      <c r="C319" t="s">
+        <v>2232</v>
+      </c>
+      <c r="D319">
+        <v>100</v>
+      </c>
+      <c r="F319" s="32">
+        <f t="shared" si="4"/>
+        <v>11632.039999999992</v>
+      </c>
+      <c r="G319" t="s">
+        <v>10</v>
+      </c>
+      <c r="H319" t="s">
+        <v>869</v>
+      </c>
+      <c r="I319" t="s">
+        <v>2234</v>
+      </c>
+    </row>
+    <row r="320" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A320" s="31">
+        <v>45566</v>
+      </c>
+      <c r="B320" t="s">
+        <v>396</v>
+      </c>
+      <c r="C320" t="s">
+        <v>2233</v>
+      </c>
+      <c r="E320">
+        <v>221.2</v>
+      </c>
+      <c r="F320" s="32">
+        <f t="shared" si="4"/>
+        <v>11853.239999999993</v>
+      </c>
+      <c r="G320" t="s">
+        <v>808</v>
+      </c>
+      <c r="H320" t="s">
         <v>870</v>
       </c>
     </row>
@@ -24830,8 +25040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAEFBAE9-58F4-4427-A222-4B6D8D551056}">
   <dimension ref="A1:P696"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="A469" workbookViewId="0">
+      <selection activeCell="A482" sqref="A482"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -43785,7 +43995,7 @@
   <dimension ref="A1:AH20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="J10" sqref="J10:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -43822,10 +44032,10 @@
       </c>
       <c r="F1"/>
       <c r="G1" s="5" t="s">
-        <v>2223</v>
+        <v>2222</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>2228</v>
+        <v>2227</v>
       </c>
       <c r="Y1"/>
       <c r="Z1"/>
@@ -43858,7 +44068,7 @@
         <v>4.2249999999999996</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>2225</v>
+        <v>2224</v>
       </c>
       <c r="I2" s="38">
         <v>1.6899999999999998E-2</v>
@@ -43885,23 +44095,23 @@
         <v>60</v>
       </c>
       <c r="D3" s="35">
-        <f t="shared" ref="D3:D11" si="0">C3*0.25</f>
+        <f t="shared" ref="D3:D14" si="0">C3*0.25</f>
         <v>15</v>
       </c>
       <c r="E3" s="35">
-        <f t="shared" ref="E3:E11" si="1">C3-D3</f>
+        <f t="shared" ref="E3:E14" si="1">C3-D3</f>
         <v>45</v>
       </c>
       <c r="F3"/>
       <c r="G3" s="37">
-        <f t="shared" ref="G3:G11" si="2">0.0169*C3</f>
+        <f t="shared" ref="G3:G14" si="2">0.0169*C3</f>
         <v>1.0139999999999998</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>2225</v>
+        <v>2224</v>
       </c>
       <c r="J3" s="37">
-        <f t="shared" ref="J3:J11" si="3">C3-G3</f>
+        <f t="shared" ref="J3:J14" si="3">C3-G3</f>
         <v>58.985999999999997</v>
       </c>
       <c r="AG3" s="2"/>
@@ -43927,7 +44137,7 @@
         <v>1.3519999999999999</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>2225</v>
+        <v>2224</v>
       </c>
       <c r="J4" s="37">
         <f t="shared" si="3"/>
@@ -43955,7 +44165,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>2227</v>
+        <v>2226</v>
       </c>
       <c r="J5" s="37">
         <f t="shared" si="3"/>
@@ -43983,7 +44193,7 @@
         <v>20.195499999999999</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>2225</v>
+        <v>2224</v>
       </c>
       <c r="J6" s="37">
         <f t="shared" si="3"/>
@@ -44011,10 +44221,10 @@
         <v>5.45</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>2224</v>
+        <v>2223</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>2226</v>
+        <v>2225</v>
       </c>
       <c r="J7" s="37">
         <f t="shared" si="3"/>
@@ -44041,11 +44251,14 @@
         <v>7.8584999999999994</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>2225</v>
+        <v>2224</v>
       </c>
       <c r="J8" s="37">
         <f t="shared" si="3"/>
         <v>457.14150000000001</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>2230</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
@@ -44068,7 +44281,7 @@
         <v>5.0699999999999994</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>2225</v>
+        <v>2224</v>
       </c>
       <c r="J9" s="37">
         <f t="shared" si="3"/>
@@ -44095,7 +44308,7 @@
         <v>7.3514999999999997</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>2225</v>
+        <v>2224</v>
       </c>
       <c r="J10" s="37">
         <f t="shared" si="3"/>
@@ -44122,7 +44335,7 @@
         <v>2.1124999999999998</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>2225</v>
+        <v>2224</v>
       </c>
       <c r="J11" s="37">
         <f t="shared" si="3"/>
@@ -44132,72 +44345,133 @@
     <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12"/>
       <c r="B12"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
+      <c r="C12" s="35">
+        <v>130</v>
+      </c>
+      <c r="D12" s="35">
+        <f t="shared" si="0"/>
+        <v>32.5</v>
+      </c>
+      <c r="E12" s="35">
+        <f t="shared" si="1"/>
+        <v>97.5</v>
+      </c>
       <c r="F12"/>
+      <c r="G12" s="37">
+        <f t="shared" si="2"/>
+        <v>2.1969999999999996</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>2224</v>
+      </c>
+      <c r="J12" s="37">
+        <f t="shared" si="3"/>
+        <v>127.803</v>
+      </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13"/>
       <c r="B13"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
+      <c r="C13" s="35">
+        <v>65</v>
+      </c>
+      <c r="D13" s="35">
+        <f t="shared" si="0"/>
+        <v>16.25</v>
+      </c>
+      <c r="E13" s="35">
+        <f t="shared" si="1"/>
+        <v>48.75</v>
+      </c>
       <c r="F13"/>
+      <c r="G13" s="37">
+        <f t="shared" si="2"/>
+        <v>1.0984999999999998</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>2224</v>
+      </c>
+      <c r="J13" s="37">
+        <f t="shared" si="3"/>
+        <v>63.901499999999999</v>
+      </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14"/>
       <c r="B14"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
+      <c r="C14" s="35">
+        <v>225</v>
+      </c>
+      <c r="D14" s="35">
+        <f t="shared" si="0"/>
+        <v>56.25</v>
+      </c>
+      <c r="E14" s="35">
+        <f t="shared" si="1"/>
+        <v>168.75</v>
+      </c>
       <c r="F14"/>
+      <c r="G14" s="37">
+        <f t="shared" si="2"/>
+        <v>3.8024999999999998</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>2224</v>
+      </c>
+      <c r="J14" s="37">
+        <f t="shared" si="3"/>
+        <v>221.19749999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="G15" s="37"/>
+      <c r="J15" s="37"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>2221</v>
+        <v>2220</v>
       </c>
       <c r="C18" s="37">
         <f>SUM(C2:C17)</f>
-        <v>3350</v>
+        <v>3770</v>
       </c>
       <c r="D18" s="37">
         <f t="shared" ref="D18:E18" si="4">SUM(D2:D17)</f>
-        <v>837.5</v>
+        <v>942.5</v>
       </c>
       <c r="E18" s="37">
         <f t="shared" si="4"/>
-        <v>2512.5</v>
+        <v>2827.5</v>
       </c>
       <c r="G18" s="37">
         <f>SUM(G2:G17)</f>
-        <v>54.628999999999998</v>
+        <v>61.727000000000004</v>
       </c>
       <c r="J18" s="37">
         <f>SUM(J2:J17)</f>
-        <v>3295.3709999999992</v>
+        <v>3708.2729999999992</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>2222</v>
+        <v>2221</v>
       </c>
       <c r="C19" s="5">
         <f>COUNT(C2:C17)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>2229</v>
+        <v>2228</v>
       </c>
       <c r="J19" s="37">
         <f>E18</f>
-        <v>2512.5</v>
+        <v>2827.5</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J20" s="39">
         <f>J18-J19</f>
-        <v>782.87099999999919</v>
+        <v>880.77299999999923</v>
       </c>
     </row>
   </sheetData>
@@ -44276,7 +44550,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -44371,7 +44645,7 @@
     </row>
     <row r="28" spans="1:1" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>2213</v>
+        <v>2212</v>
       </c>
     </row>
   </sheetData>
@@ -48956,7 +49230,7 @@
         <v>825</v>
       </c>
       <c r="C11" t="s">
-        <v>2211</v>
+        <v>2210</v>
       </c>
       <c r="E11">
         <v>27.26</v>
@@ -48974,10 +49248,10 @@
         <v>45560</v>
       </c>
       <c r="B12" t="s">
-        <v>2209</v>
+        <v>2208</v>
       </c>
       <c r="C12" t="s">
-        <v>2212</v>
+        <v>2211</v>
       </c>
       <c r="E12">
         <v>6000</v>
@@ -49011,7 +49285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEAEDB9-0FE6-48E6-8096-45942EADC73F}">
   <dimension ref="A3:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -49251,7 +49525,8 @@
       <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="B4" s="40"/>
+      <c r="C4" s="40">
         <v>495.98</v>
       </c>
       <c r="E4" s="33" t="s">
@@ -49268,33 +49543,35 @@
       <c r="A5" s="34" t="s">
         <v>812</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="40">
         <v>100.98</v>
       </c>
+      <c r="C5" s="40"/>
       <c r="E5" s="34" t="s">
         <v>869</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="40">
         <v>6507.65</v>
       </c>
-      <c r="G5">
-        <v>6619.18</v>
+      <c r="G5" s="40">
+        <v>6719.18</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C6">
-        <v>700</v>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40">
+        <v>800</v>
       </c>
       <c r="E6" s="34" t="s">
         <v>870</v>
       </c>
-      <c r="F6">
-        <v>10524.350000000002</v>
-      </c>
-      <c r="G6">
+      <c r="F6" s="40">
+        <v>11832.340000000002</v>
+      </c>
+      <c r="G6" s="40">
         <v>780</v>
       </c>
     </row>
@@ -49302,16 +49579,17 @@
       <c r="A7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C7">
+      <c r="B7" s="40"/>
+      <c r="C7" s="40">
         <v>916.6</v>
       </c>
       <c r="E7" s="34" t="s">
         <v>574</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="40">
         <v>7449.9100000000008</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="40">
         <v>11467.09</v>
       </c>
     </row>
@@ -49319,32 +49597,35 @@
       <c r="A8" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C8">
+      <c r="B8" s="40"/>
+      <c r="C8" s="40">
         <v>361</v>
       </c>
       <c r="E8" s="34" t="s">
         <v>573</v>
       </c>
-      <c r="F8">
-        <v>24481.91</v>
-      </c>
-      <c r="G8">
-        <v>18866.27</v>
+      <c r="F8" s="40">
+        <v>25789.9</v>
+      </c>
+      <c r="G8" s="40">
+        <v>18966.27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>808</v>
       </c>
-      <c r="B9">
-        <v>6023.96</v>
-      </c>
+      <c r="B9" s="40">
+        <v>7331.95</v>
+      </c>
+      <c r="C9" s="40"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
         <v>809</v>
       </c>
-      <c r="C10">
+      <c r="B10" s="40"/>
+      <c r="C10" s="40">
         <v>2632.5</v>
       </c>
     </row>
@@ -49352,15 +49633,17 @@
       <c r="A11" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="40">
         <v>7447.9500000000016</v>
       </c>
+      <c r="C11" s="40"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C12">
+      <c r="B12" s="40"/>
+      <c r="C12" s="40">
         <v>481.52</v>
       </c>
     </row>
@@ -49368,7 +49651,8 @@
       <c r="A13" s="34" t="s">
         <v>810</v>
       </c>
-      <c r="C13">
+      <c r="B13" s="40"/>
+      <c r="C13" s="40">
         <v>1100</v>
       </c>
     </row>
@@ -49376,20 +49660,24 @@
       <c r="A14" s="34" t="s">
         <v>574</v>
       </c>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="40">
         <v>10612.48</v>
       </c>
+      <c r="C15" s="40"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="C16">
+      <c r="B16" s="40"/>
+      <c r="C16" s="40">
         <v>773</v>
       </c>
     </row>
@@ -49397,7 +49685,8 @@
       <c r="A17" s="34" t="s">
         <v>864</v>
       </c>
-      <c r="C17">
+      <c r="B17" s="40"/>
+      <c r="C17" s="40">
         <v>1500</v>
       </c>
     </row>
@@ -49405,7 +49694,8 @@
       <c r="A18" s="34" t="s">
         <v>861</v>
       </c>
-      <c r="C18">
+      <c r="B18" s="40"/>
+      <c r="C18" s="40">
         <v>156.19999999999999</v>
       </c>
     </row>
@@ -49413,7 +49703,8 @@
       <c r="A19" s="34" t="s">
         <v>862</v>
       </c>
-      <c r="C19">
+      <c r="B19" s="40"/>
+      <c r="C19" s="40">
         <v>137.44999999999999</v>
       </c>
     </row>
@@ -49421,7 +49712,8 @@
       <c r="A20" s="34" t="s">
         <v>858</v>
       </c>
-      <c r="C20">
+      <c r="B20" s="40"/>
+      <c r="C20" s="40">
         <v>614.34</v>
       </c>
     </row>
@@ -49429,7 +49721,8 @@
       <c r="A21" s="34" t="s">
         <v>863</v>
       </c>
-      <c r="C21">
+      <c r="B21" s="40"/>
+      <c r="C21" s="40">
         <v>1261.68</v>
       </c>
     </row>
@@ -49437,23 +49730,26 @@
       <c r="A22" s="34" t="s">
         <v>929</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="40">
         <v>0.98</v>
       </c>
+      <c r="C22" s="40"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
         <v>811</v>
       </c>
-      <c r="C23">
+      <c r="B23" s="40"/>
+      <c r="C23" s="40">
         <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
-        <v>2213</v>
-      </c>
-      <c r="C24">
+        <v>2212</v>
+      </c>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40">
         <v>1500</v>
       </c>
     </row>
@@ -49461,23 +49757,26 @@
       <c r="A25" s="34" t="s">
         <v>930</v>
       </c>
-      <c r="C25">
+      <c r="B25" s="40"/>
+      <c r="C25" s="40">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="34" t="s">
-        <v>2208</v>
-      </c>
-      <c r="B26">
+        <v>2207</v>
+      </c>
+      <c r="B26" s="40">
         <v>295.56</v>
       </c>
+      <c r="C26" s="40"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C27">
+      <c r="B27" s="40"/>
+      <c r="C27" s="40">
         <v>6000</v>
       </c>
     </row>
@@ -49485,11 +49784,11 @@
       <c r="A28" s="34" t="s">
         <v>573</v>
       </c>
-      <c r="B28">
-        <v>24481.910000000003</v>
-      </c>
-      <c r="C28">
-        <v>18866.270000000004</v>
+      <c r="B28" s="40">
+        <v>25789.9</v>
+      </c>
+      <c r="C28" s="40">
+        <v>18966.270000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add sales email merge
</commit_message>
<xml_diff>
--- a/2024/OAS 2024.xlsx
+++ b/2024/OAS 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnbar\Dropbox\OAS\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86880FFB-0569-4D8C-BA13-69DD543AF1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8966A7-26FF-4D69-A0B5-D4123500F4B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="7" activeTab="8" xr2:uid="{E6A7689A-682B-425D-92A3-B87F804748A5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10800" firstSheet="8" activeTab="8" xr2:uid="{E6A7689A-682B-425D-92A3-B87F804748A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="8" r:id="rId1"/>
@@ -29,10 +29,10 @@
     <sheet name="Open Exhibition" sheetId="6" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Current account'!$A$1:$I$313</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Current account'!$A$1:$I$323</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Stripe!$A$1:$P$481</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId15"/>
     <pivotCache cacheId="7" r:id="rId16"/>
@@ -49,6 +49,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -56,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4813" uniqueCount="2235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4900" uniqueCount="2254">
   <si>
     <t>Subs</t>
   </si>
@@ -6761,6 +6763,63 @@
   </si>
   <si>
     <t xml:space="preserve">Prizewinner forgot to cash cheque </t>
+  </si>
+  <si>
+    <t>SumUp Payments AccMDD PID741362</t>
+  </si>
+  <si>
+    <t>SumUp Payments AccMDD PID743225</t>
+  </si>
+  <si>
+    <t>SumUp Payments AccMDD PID748134</t>
+  </si>
+  <si>
+    <t>Vivian Shelton OAS</t>
+  </si>
+  <si>
+    <t>Mrs C E Hopton OAS</t>
+  </si>
+  <si>
+    <t>Miranda Miller OAS</t>
+  </si>
+  <si>
+    <t>Anna Kolos OAS</t>
+  </si>
+  <si>
+    <t>Peter Collins OAS</t>
+  </si>
+  <si>
+    <t>Melinda Kenneway OAS</t>
+  </si>
+  <si>
+    <t>Claire Drinkwater OAS</t>
+  </si>
+  <si>
+    <t>John Day OAS</t>
+  </si>
+  <si>
+    <t>Hannah Farncombe OAS</t>
+  </si>
+  <si>
+    <t>Harriet Calfo OAS</t>
+  </si>
+  <si>
+    <t>June Dent OAS</t>
+  </si>
+  <si>
+    <t>Gerry Coles PrintsOAS</t>
+  </si>
+  <si>
+    <t>Eirian Griffiths OAS</t>
+  </si>
+  <si>
+    <t>Rod Craig OAS</t>
+  </si>
+  <si>
+    <t>Tereza Horacek OAS</t>
+  </si>
+  <si>
+    <t>Lizzie Wheeler OAS</t>
   </si>
 </sst>
 </file>
@@ -7025,13 +7084,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45567.394030324074" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="320" xr:uid="{52AA0CD4-A3EB-4892-953B-4445B6BC29AB}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45575.635887037039" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="340" xr:uid="{52AA0CD4-A3EB-4892-953B-4445B6BC29AB}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I502" sheet="Current account"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2024-01-01T00:00:00" maxDate="2024-10-02T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2024-01-01T00:00:00" maxDate="2024-10-11T00:00:00"/>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -7043,7 +7102,7 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5" maxValue="6000"/>
     </cacheField>
     <cacheField name="Income" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.98" maxValue="2097.8000000000002"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.98" maxValue="2949.3"/>
     </cacheField>
     <cacheField name="Balance" numFmtId="164">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5059.6099999999997" maxValue="17759.57"/>
@@ -7055,6 +7114,7 @@
         <s v="Submissions"/>
         <s v="Website"/>
         <s v="Donations cr"/>
+        <s v="Other income"/>
         <s v="Bar sales"/>
         <s v="Sales cr"/>
         <s v="Prizes"/>
@@ -7069,7 +7129,6 @@
         <s v="Venue hire"/>
         <s v="Gifts"/>
         <s v="Insurance"/>
-        <s v="Other income"/>
         <s v="Exhibitions db"/>
         <s v="Other expenses"/>
         <s v="Transfer Out"/>
@@ -7096,13 +7155,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45567.394124768522" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="320" xr:uid="{133830F7-3A79-4A2B-AFB2-D11D3864E8D7}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45575.635936921295" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="340" xr:uid="{133830F7-3A79-4A2B-AFB2-D11D3864E8D7}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:H501" sheet="Current account"/>
   </cacheSource>
   <cacheFields count="8">
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2024-01-01T00:00:00" maxDate="2024-10-02T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2024-01-01T00:00:00" maxDate="2024-10-11T00:00:00"/>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -7114,7 +7173,7 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5" maxValue="6000"/>
     </cacheField>
     <cacheField name="Income" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.98" maxValue="2097.8000000000002"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.98" maxValue="2949.3"/>
     </cacheField>
     <cacheField name="Balance" numFmtId="164">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5059.6099999999997" maxValue="17759.57"/>
@@ -7126,6 +7185,7 @@
         <s v="Submissions"/>
         <s v="Website"/>
         <s v="Donations cr"/>
+        <s v="Other income"/>
         <s v="Bar sales"/>
         <s v="Sales cr"/>
         <s v="Prizes"/>
@@ -7140,7 +7200,6 @@
         <s v="Venue hire"/>
         <s v="Gifts"/>
         <s v="Insurance"/>
-        <s v="Other income"/>
         <s v="Exhibitions db"/>
         <s v="Other expenses"/>
         <s v="Transfer Out"/>
@@ -9064,7 +9123,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="320">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="340">
   <r>
     <d v="2024-01-01T00:00:00"/>
     <s v="CR"/>
@@ -11338,7 +11397,7 @@
     <m/>
     <n v="0.98"/>
     <n v="14627.1"/>
-    <x v="4"/>
+    <x v="5"/>
     <x v="0"/>
     <m/>
   </r>
@@ -11349,7 +11408,7 @@
     <m/>
     <n v="178.99"/>
     <n v="14806.09"/>
-    <x v="5"/>
+    <x v="6"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11360,7 +11419,7 @@
     <m/>
     <n v="663.59"/>
     <n v="15469.68"/>
-    <x v="6"/>
+    <x v="7"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11371,7 +11430,7 @@
     <m/>
     <n v="324.42"/>
     <n v="15794.1"/>
-    <x v="6"/>
+    <x v="7"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11382,7 +11441,7 @@
     <m/>
     <n v="344.4"/>
     <n v="16138.5"/>
-    <x v="6"/>
+    <x v="7"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11393,7 +11452,7 @@
     <m/>
     <n v="580.02"/>
     <n v="16718.52"/>
-    <x v="6"/>
+    <x v="7"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11404,7 +11463,7 @@
     <m/>
     <n v="663.59"/>
     <n v="17382.11"/>
-    <x v="6"/>
+    <x v="7"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11415,7 +11474,7 @@
     <m/>
     <n v="304.76"/>
     <n v="17686.87"/>
-    <x v="6"/>
+    <x v="7"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11426,7 +11485,7 @@
     <n v="100"/>
     <m/>
     <n v="17586.87"/>
-    <x v="7"/>
+    <x v="8"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11437,7 +11496,7 @@
     <m/>
     <n v="172.7"/>
     <n v="17759.57"/>
-    <x v="6"/>
+    <x v="7"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11459,7 +11518,7 @@
     <n v="1500"/>
     <m/>
     <n v="16195.59"/>
-    <x v="8"/>
+    <x v="9"/>
     <x v="0"/>
     <s v="Payment to web manager"/>
   </r>
@@ -11470,7 +11529,7 @@
     <n v="175"/>
     <m/>
     <n v="16020.59"/>
-    <x v="9"/>
+    <x v="10"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11481,7 +11540,7 @@
     <n v="1500"/>
     <m/>
     <n v="14520.59"/>
-    <x v="10"/>
+    <x v="11"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11492,7 +11551,7 @@
     <m/>
     <n v="570.20000000000005"/>
     <n v="15090.79"/>
-    <x v="6"/>
+    <x v="7"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11503,7 +11562,7 @@
     <n v="100"/>
     <m/>
     <n v="14990.79"/>
-    <x v="7"/>
+    <x v="8"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11514,7 +11573,7 @@
     <n v="175"/>
     <m/>
     <n v="14815.79"/>
-    <x v="11"/>
+    <x v="12"/>
     <x v="1"/>
     <s v="Painting sold twice!"/>
   </r>
@@ -11525,7 +11584,7 @@
     <n v="100"/>
     <m/>
     <n v="14715.79"/>
-    <x v="7"/>
+    <x v="8"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11536,7 +11595,7 @@
     <n v="100"/>
     <m/>
     <n v="14615.79"/>
-    <x v="7"/>
+    <x v="8"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11558,7 +11617,7 @@
     <n v="916.6"/>
     <m/>
     <n v="13694.19"/>
-    <x v="12"/>
+    <x v="13"/>
     <x v="0"/>
     <m/>
   </r>
@@ -11580,7 +11639,7 @@
     <n v="375"/>
     <m/>
     <n v="12929.19"/>
-    <x v="9"/>
+    <x v="10"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11591,7 +11650,7 @@
     <n v="262.5"/>
     <m/>
     <n v="12666.69"/>
-    <x v="13"/>
+    <x v="14"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11602,7 +11661,7 @@
     <n v="232.5"/>
     <m/>
     <n v="12434.19"/>
-    <x v="13"/>
+    <x v="14"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11613,7 +11672,7 @@
     <n v="131.25"/>
     <m/>
     <n v="12302.94"/>
-    <x v="13"/>
+    <x v="14"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11624,7 +11683,7 @@
     <n v="187.5"/>
     <m/>
     <n v="12115.44"/>
-    <x v="13"/>
+    <x v="14"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11635,7 +11694,7 @@
     <n v="221.25"/>
     <m/>
     <n v="11894.19"/>
-    <x v="13"/>
+    <x v="14"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11646,7 +11705,7 @@
     <n v="221.25"/>
     <m/>
     <n v="11672.94"/>
-    <x v="13"/>
+    <x v="14"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11657,7 +11716,7 @@
     <n v="247.5"/>
     <m/>
     <n v="11425.44"/>
-    <x v="13"/>
+    <x v="14"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11668,7 +11727,7 @@
     <n v="435"/>
     <m/>
     <n v="10990.44"/>
-    <x v="13"/>
+    <x v="14"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11679,7 +11738,7 @@
     <n v="318.75"/>
     <m/>
     <n v="10671.69"/>
-    <x v="13"/>
+    <x v="14"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11690,7 +11749,7 @@
     <n v="285"/>
     <m/>
     <n v="10386.69"/>
-    <x v="13"/>
+    <x v="14"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11701,7 +11760,7 @@
     <n v="90"/>
     <m/>
     <n v="10296.69"/>
-    <x v="13"/>
+    <x v="14"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11789,7 +11848,7 @@
     <n v="156.19999999999999"/>
     <m/>
     <n v="10337.239999999996"/>
-    <x v="14"/>
+    <x v="15"/>
     <x v="0"/>
     <s v="AGM drinks"/>
   </r>
@@ -11800,7 +11859,7 @@
     <n v="30"/>
     <m/>
     <n v="10307.239999999996"/>
-    <x v="11"/>
+    <x v="12"/>
     <x v="0"/>
     <m/>
   </r>
@@ -11811,7 +11870,7 @@
     <n v="30"/>
     <m/>
     <n v="10277.239999999996"/>
-    <x v="11"/>
+    <x v="12"/>
     <x v="0"/>
     <m/>
   </r>
@@ -11844,7 +11903,7 @@
     <n v="50"/>
     <m/>
     <n v="10049.739999999996"/>
-    <x v="15"/>
+    <x v="16"/>
     <x v="0"/>
     <m/>
   </r>
@@ -11855,7 +11914,7 @@
     <n v="400"/>
     <m/>
     <n v="9649.7399999999961"/>
-    <x v="15"/>
+    <x v="16"/>
     <x v="0"/>
     <m/>
   </r>
@@ -11877,7 +11936,7 @@
     <n v="100"/>
     <m/>
     <n v="9578.7899999999954"/>
-    <x v="7"/>
+    <x v="8"/>
     <x v="1"/>
     <m/>
   </r>
@@ -11899,7 +11958,7 @@
     <n v="1261.68"/>
     <m/>
     <n v="8312.1099999999951"/>
-    <x v="16"/>
+    <x v="17"/>
     <x v="1"/>
     <s v="Includes catering"/>
   </r>
@@ -12031,7 +12090,7 @@
     <n v="18.5"/>
     <m/>
     <n v="9078.7499999999945"/>
-    <x v="17"/>
+    <x v="18"/>
     <x v="0"/>
     <s v="Gift to John"/>
   </r>
@@ -12086,7 +12145,7 @@
     <n v="614.34"/>
     <m/>
     <n v="8837.389999999994"/>
-    <x v="18"/>
+    <x v="19"/>
     <x v="0"/>
     <m/>
   </r>
@@ -12229,7 +12288,7 @@
     <n v="223"/>
     <m/>
     <n v="11045.379999999994"/>
-    <x v="9"/>
+    <x v="10"/>
     <x v="2"/>
     <m/>
   </r>
@@ -12361,7 +12420,7 @@
     <n v="108"/>
     <m/>
     <n v="15320.369999999995"/>
-    <x v="11"/>
+    <x v="12"/>
     <x v="2"/>
     <m/>
   </r>
@@ -12383,7 +12442,7 @@
     <m/>
     <n v="0.98"/>
     <n v="15351.349999999995"/>
-    <x v="19"/>
+    <x v="5"/>
     <x v="0"/>
     <m/>
   </r>
@@ -12416,7 +12475,7 @@
     <m/>
     <n v="90"/>
     <n v="15210.349999999995"/>
-    <x v="6"/>
+    <x v="7"/>
     <x v="2"/>
     <m/>
   </r>
@@ -12438,7 +12497,7 @@
     <m/>
     <n v="116.57"/>
     <n v="15321.919999999995"/>
-    <x v="5"/>
+    <x v="6"/>
     <x v="2"/>
     <m/>
   </r>
@@ -12449,7 +12508,7 @@
     <m/>
     <n v="1558.21"/>
     <n v="16880.129999999994"/>
-    <x v="6"/>
+    <x v="7"/>
     <x v="2"/>
     <m/>
   </r>
@@ -12471,7 +12530,7 @@
     <n v="18"/>
     <m/>
     <n v="10862.129999999994"/>
-    <x v="11"/>
+    <x v="12"/>
     <x v="2"/>
     <m/>
   </r>
@@ -12482,7 +12541,7 @@
     <n v="118.95"/>
     <m/>
     <n v="10743.179999999993"/>
-    <x v="17"/>
+    <x v="18"/>
     <x v="0"/>
     <m/>
   </r>
@@ -12493,7 +12552,7 @@
     <m/>
     <n v="457.14"/>
     <n v="11200.319999999992"/>
-    <x v="6"/>
+    <x v="7"/>
     <x v="2"/>
     <m/>
   </r>
@@ -12504,7 +12563,7 @@
     <n v="650"/>
     <m/>
     <n v="10550.319999999992"/>
-    <x v="15"/>
+    <x v="16"/>
     <x v="0"/>
     <m/>
   </r>
@@ -12515,19 +12574,19 @@
     <n v="200"/>
     <m/>
     <n v="10350.319999999992"/>
+    <x v="8"/>
+    <x v="2"/>
+    <s v="Reimbursement "/>
+  </r>
+  <r>
+    <d v="2024-09-27T00:00:00"/>
+    <s v="CR"/>
+    <s v="SumUp Payments AccMDD PID731586"/>
+    <m/>
+    <n v="294.93"/>
+    <n v="10645.249999999993"/>
     <x v="7"/>
     <x v="2"/>
-    <s v="Reimbursement "/>
-  </r>
-  <r>
-    <d v="2024-09-27T00:00:00"/>
-    <s v="CR"/>
-    <s v="SumUp Payments AccMDD PID731586"/>
-    <m/>
-    <n v="294.93"/>
-    <n v="10645.249999999993"/>
-    <x v="6"/>
-    <x v="2"/>
     <m/>
   </r>
   <r>
@@ -12537,7 +12596,7 @@
     <m/>
     <n v="344.55"/>
     <n v="10989.799999999992"/>
-    <x v="6"/>
+    <x v="7"/>
     <x v="2"/>
     <m/>
   </r>
@@ -12548,7 +12607,7 @@
     <m/>
     <n v="742.24"/>
     <n v="11732.039999999992"/>
-    <x v="6"/>
+    <x v="7"/>
     <x v="2"/>
     <m/>
   </r>
@@ -12559,7 +12618,7 @@
     <n v="100"/>
     <m/>
     <n v="11632.039999999992"/>
-    <x v="7"/>
+    <x v="8"/>
     <x v="1"/>
     <s v="Prizewinner forgot to cash cheque "/>
   </r>
@@ -12570,8 +12629,228 @@
     <m/>
     <n v="221.2"/>
     <n v="11853.239999999993"/>
-    <x v="6"/>
+    <x v="7"/>
     <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-03T00:00:00"/>
+    <s v="CR"/>
+    <s v="SumUp Payments AccMDD PID741362"/>
+    <m/>
+    <n v="879.87"/>
+    <n v="12733.109999999993"/>
+    <x v="7"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-04T00:00:00"/>
+    <s v="CR"/>
+    <s v="SumUp Payments AccMDD PID743225"/>
+    <m/>
+    <n v="2949.3"/>
+    <n v="15682.409999999993"/>
+    <x v="7"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-07T00:00:00"/>
+    <s v="CR"/>
+    <s v="SumUp Payments AccMDD PID748134"/>
+    <m/>
+    <n v="1327.17"/>
+    <n v="17009.579999999994"/>
+    <x v="7"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-08T00:00:00"/>
+    <s v="BP"/>
+    <s v="Vivian Shelton OAS"/>
+    <n v="112.87"/>
+    <m/>
+    <n v="16896.709999999995"/>
+    <x v="20"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Mrs C E Hopton OAS"/>
+    <n v="45"/>
+    <m/>
+    <n v="16851.709999999995"/>
+    <x v="14"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Miranda Miller OAS"/>
+    <n v="60"/>
+    <m/>
+    <n v="16791.709999999995"/>
+    <x v="14"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Anna Kolos OAS"/>
+    <n v="262.5"/>
+    <m/>
+    <n v="16529.209999999995"/>
+    <x v="14"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Peter Collins OAS"/>
+    <n v="67.5"/>
+    <m/>
+    <n v="16461.709999999995"/>
+    <x v="14"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Melinda Kenneway OAS"/>
+    <n v="896.25"/>
+    <m/>
+    <n v="15565.459999999995"/>
+    <x v="14"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Claire Drinkwater OAS"/>
+    <n v="93.75"/>
+    <m/>
+    <n v="15471.709999999995"/>
+    <x v="14"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="John Day OAS"/>
+    <n v="108.75"/>
+    <m/>
+    <n v="15362.959999999995"/>
+    <x v="14"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Hannah Farncombe OAS"/>
+    <n v="168.75"/>
+    <m/>
+    <n v="15194.209999999995"/>
+    <x v="14"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Harriet Calfo OAS"/>
+    <n v="262.5"/>
+    <m/>
+    <n v="14931.709999999995"/>
+    <x v="14"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="June Dent OAS"/>
+    <n v="221.25"/>
+    <m/>
+    <n v="14710.459999999995"/>
+    <x v="14"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Gerry Coles PrintsOAS"/>
+    <n v="48.75"/>
+    <m/>
+    <n v="14661.709999999995"/>
+    <x v="14"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Eirian Griffiths OAS"/>
+    <n v="172.5"/>
+    <m/>
+    <n v="14489.209999999995"/>
+    <x v="14"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Rod Craig OAS"/>
+    <n v="671.25"/>
+    <m/>
+    <n v="13817.959999999995"/>
+    <x v="14"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-10T00:00:00"/>
+    <s v="BP"/>
+    <s v="Tereza Horacek OAS"/>
+    <n v="187.5"/>
+    <m/>
+    <n v="13630.459999999995"/>
+    <x v="14"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-10T00:00:00"/>
+    <s v="BP"/>
+    <s v="Lizzie Wheeler OAS"/>
+    <n v="240"/>
+    <m/>
+    <n v="13390.459999999995"/>
+    <x v="14"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2024-10-10T00:00:00"/>
+    <s v="CR"/>
+    <s v="Stripe Payments UKSTRIPE"/>
+    <m/>
+    <n v="29.2"/>
+    <n v="13419.659999999996"/>
+    <x v="0"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -12589,7 +12868,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="320">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="340">
   <r>
     <d v="2024-01-01T00:00:00"/>
     <s v="CR"/>
@@ -14657,7 +14936,7 @@
     <m/>
     <n v="0.98"/>
     <n v="14627.1"/>
-    <x v="4"/>
+    <x v="5"/>
     <m/>
   </r>
   <r>
@@ -14667,7 +14946,7 @@
     <m/>
     <n v="178.99"/>
     <n v="14806.09"/>
-    <x v="5"/>
+    <x v="6"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14677,7 +14956,7 @@
     <m/>
     <n v="663.59"/>
     <n v="15469.68"/>
-    <x v="6"/>
+    <x v="7"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14687,7 +14966,7 @@
     <m/>
     <n v="324.42"/>
     <n v="15794.1"/>
-    <x v="6"/>
+    <x v="7"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14697,7 +14976,7 @@
     <m/>
     <n v="344.4"/>
     <n v="16138.5"/>
-    <x v="6"/>
+    <x v="7"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14707,7 +14986,7 @@
     <m/>
     <n v="580.02"/>
     <n v="16718.52"/>
-    <x v="6"/>
+    <x v="7"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14717,7 +14996,7 @@
     <m/>
     <n v="663.59"/>
     <n v="17382.11"/>
-    <x v="6"/>
+    <x v="7"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14727,7 +15006,7 @@
     <m/>
     <n v="304.76"/>
     <n v="17686.87"/>
-    <x v="6"/>
+    <x v="7"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14737,7 +15016,7 @@
     <n v="100"/>
     <m/>
     <n v="17586.87"/>
-    <x v="7"/>
+    <x v="8"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14747,7 +15026,7 @@
     <m/>
     <n v="172.7"/>
     <n v="17759.57"/>
-    <x v="6"/>
+    <x v="7"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14767,7 +15046,7 @@
     <n v="1500"/>
     <m/>
     <n v="16195.59"/>
-    <x v="8"/>
+    <x v="9"/>
     <m/>
   </r>
   <r>
@@ -14777,7 +15056,7 @@
     <n v="175"/>
     <m/>
     <n v="16020.59"/>
-    <x v="9"/>
+    <x v="10"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14787,7 +15066,7 @@
     <n v="1500"/>
     <m/>
     <n v="14520.59"/>
-    <x v="10"/>
+    <x v="11"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14797,7 +15076,7 @@
     <m/>
     <n v="570.20000000000005"/>
     <n v="15090.79"/>
-    <x v="6"/>
+    <x v="7"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14807,7 +15086,7 @@
     <n v="100"/>
     <m/>
     <n v="14990.79"/>
-    <x v="7"/>
+    <x v="8"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14817,7 +15096,7 @@
     <n v="175"/>
     <m/>
     <n v="14815.79"/>
-    <x v="11"/>
+    <x v="12"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14827,7 +15106,7 @@
     <n v="100"/>
     <m/>
     <n v="14715.79"/>
-    <x v="7"/>
+    <x v="8"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14837,7 +15116,7 @@
     <n v="100"/>
     <m/>
     <n v="14615.79"/>
-    <x v="7"/>
+    <x v="8"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14857,7 +15136,7 @@
     <n v="916.6"/>
     <m/>
     <n v="13694.19"/>
-    <x v="12"/>
+    <x v="13"/>
     <m/>
   </r>
   <r>
@@ -14877,7 +15156,7 @@
     <n v="375"/>
     <m/>
     <n v="12929.19"/>
-    <x v="9"/>
+    <x v="10"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14887,7 +15166,7 @@
     <n v="262.5"/>
     <m/>
     <n v="12666.69"/>
-    <x v="13"/>
+    <x v="14"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14897,7 +15176,7 @@
     <n v="232.5"/>
     <m/>
     <n v="12434.19"/>
-    <x v="13"/>
+    <x v="14"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14907,7 +15186,7 @@
     <n v="131.25"/>
     <m/>
     <n v="12302.94"/>
-    <x v="13"/>
+    <x v="14"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14917,7 +15196,7 @@
     <n v="187.5"/>
     <m/>
     <n v="12115.44"/>
-    <x v="13"/>
+    <x v="14"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14927,7 +15206,7 @@
     <n v="221.25"/>
     <m/>
     <n v="11894.19"/>
-    <x v="13"/>
+    <x v="14"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14937,7 +15216,7 @@
     <n v="221.25"/>
     <m/>
     <n v="11672.94"/>
-    <x v="13"/>
+    <x v="14"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14947,7 +15226,7 @@
     <n v="247.5"/>
     <m/>
     <n v="11425.44"/>
-    <x v="13"/>
+    <x v="14"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14957,7 +15236,7 @@
     <n v="435"/>
     <m/>
     <n v="10990.44"/>
-    <x v="13"/>
+    <x v="14"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14967,7 +15246,7 @@
     <n v="318.75"/>
     <m/>
     <n v="10671.69"/>
-    <x v="13"/>
+    <x v="14"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14977,7 +15256,7 @@
     <n v="285"/>
     <m/>
     <n v="10386.69"/>
-    <x v="13"/>
+    <x v="14"/>
     <s v="Members"/>
   </r>
   <r>
@@ -14987,7 +15266,7 @@
     <n v="90"/>
     <m/>
     <n v="10296.69"/>
-    <x v="13"/>
+    <x v="14"/>
     <s v="Members"/>
   </r>
   <r>
@@ -15067,7 +15346,7 @@
     <n v="156.19999999999999"/>
     <m/>
     <n v="10337.239999999996"/>
-    <x v="14"/>
+    <x v="15"/>
     <m/>
   </r>
   <r>
@@ -15077,7 +15356,7 @@
     <n v="30"/>
     <m/>
     <n v="10307.239999999996"/>
-    <x v="11"/>
+    <x v="12"/>
     <m/>
   </r>
   <r>
@@ -15087,7 +15366,7 @@
     <n v="30"/>
     <m/>
     <n v="10277.239999999996"/>
-    <x v="11"/>
+    <x v="12"/>
     <m/>
   </r>
   <r>
@@ -15117,7 +15396,7 @@
     <n v="50"/>
     <m/>
     <n v="10049.739999999996"/>
-    <x v="15"/>
+    <x v="16"/>
     <m/>
   </r>
   <r>
@@ -15127,7 +15406,7 @@
     <n v="400"/>
     <m/>
     <n v="9649.7399999999961"/>
-    <x v="15"/>
+    <x v="16"/>
     <m/>
   </r>
   <r>
@@ -15147,7 +15426,7 @@
     <n v="100"/>
     <m/>
     <n v="9578.7899999999954"/>
-    <x v="7"/>
+    <x v="8"/>
     <s v="Members"/>
   </r>
   <r>
@@ -15167,7 +15446,7 @@
     <n v="1261.68"/>
     <m/>
     <n v="8312.1099999999951"/>
-    <x v="16"/>
+    <x v="17"/>
     <s v="Members"/>
   </r>
   <r>
@@ -15287,7 +15566,7 @@
     <n v="18.5"/>
     <m/>
     <n v="9078.7499999999945"/>
-    <x v="17"/>
+    <x v="18"/>
     <m/>
   </r>
   <r>
@@ -15337,7 +15616,7 @@
     <n v="614.34"/>
     <m/>
     <n v="8837.389999999994"/>
-    <x v="18"/>
+    <x v="19"/>
     <m/>
   </r>
   <r>
@@ -15467,7 +15746,7 @@
     <n v="223"/>
     <m/>
     <n v="11045.379999999994"/>
-    <x v="9"/>
+    <x v="10"/>
     <s v="Open"/>
   </r>
   <r>
@@ -15587,7 +15866,7 @@
     <n v="108"/>
     <m/>
     <n v="15320.369999999995"/>
-    <x v="11"/>
+    <x v="12"/>
     <s v="Open"/>
   </r>
   <r>
@@ -15607,7 +15886,7 @@
     <m/>
     <n v="0.98"/>
     <n v="15351.349999999995"/>
-    <x v="19"/>
+    <x v="5"/>
     <m/>
   </r>
   <r>
@@ -15637,7 +15916,7 @@
     <m/>
     <n v="90"/>
     <n v="15210.349999999995"/>
-    <x v="6"/>
+    <x v="7"/>
     <s v="Open"/>
   </r>
   <r>
@@ -15657,7 +15936,7 @@
     <m/>
     <n v="116.57"/>
     <n v="15321.919999999995"/>
-    <x v="5"/>
+    <x v="6"/>
     <s v="Open"/>
   </r>
   <r>
@@ -15667,7 +15946,7 @@
     <m/>
     <n v="1558.21"/>
     <n v="16880.129999999994"/>
-    <x v="6"/>
+    <x v="7"/>
     <s v="Open"/>
   </r>
   <r>
@@ -15687,7 +15966,7 @@
     <n v="18"/>
     <m/>
     <n v="10862.129999999994"/>
-    <x v="11"/>
+    <x v="12"/>
     <s v="Open"/>
   </r>
   <r>
@@ -15697,7 +15976,7 @@
     <n v="118.95"/>
     <m/>
     <n v="10743.179999999993"/>
-    <x v="17"/>
+    <x v="18"/>
     <m/>
   </r>
   <r>
@@ -15707,7 +15986,7 @@
     <m/>
     <n v="457.14"/>
     <n v="11200.319999999992"/>
-    <x v="6"/>
+    <x v="7"/>
     <s v="Open"/>
   </r>
   <r>
@@ -15717,7 +15996,7 @@
     <n v="650"/>
     <m/>
     <n v="10550.319999999992"/>
-    <x v="15"/>
+    <x v="16"/>
     <m/>
   </r>
   <r>
@@ -15727,27 +16006,27 @@
     <n v="200"/>
     <m/>
     <n v="10350.319999999992"/>
+    <x v="8"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-09-27T00:00:00"/>
+    <s v="CR"/>
+    <s v="SumUp Payments AccMDD PID731586"/>
+    <m/>
+    <n v="294.93"/>
+    <n v="10645.249999999993"/>
     <x v="7"/>
     <s v="Open"/>
   </r>
   <r>
-    <d v="2024-09-27T00:00:00"/>
-    <s v="CR"/>
-    <s v="SumUp Payments AccMDD PID731586"/>
-    <m/>
-    <n v="294.93"/>
-    <n v="10645.249999999993"/>
-    <x v="6"/>
-    <s v="Open"/>
-  </r>
-  <r>
     <d v="2024-09-30T00:00:00"/>
     <s v="CR"/>
     <s v="Stripe Payments UKSTRIPE"/>
     <m/>
     <n v="344.55"/>
     <n v="10989.799999999992"/>
-    <x v="6"/>
+    <x v="7"/>
     <s v="Open"/>
   </r>
   <r>
@@ -15757,7 +16036,7 @@
     <m/>
     <n v="742.24"/>
     <n v="11732.039999999992"/>
-    <x v="6"/>
+    <x v="7"/>
     <s v="Open"/>
   </r>
   <r>
@@ -15767,7 +16046,7 @@
     <n v="100"/>
     <m/>
     <n v="11632.039999999992"/>
-    <x v="7"/>
+    <x v="8"/>
     <s v="Members"/>
   </r>
   <r>
@@ -15777,8 +16056,208 @@
     <m/>
     <n v="221.2"/>
     <n v="11853.239999999993"/>
-    <x v="6"/>
+    <x v="7"/>
     <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-03T00:00:00"/>
+    <s v="CR"/>
+    <s v="SumUp Payments AccMDD PID741362"/>
+    <m/>
+    <n v="879.87"/>
+    <n v="12733.109999999993"/>
+    <x v="7"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-04T00:00:00"/>
+    <s v="CR"/>
+    <s v="SumUp Payments AccMDD PID743225"/>
+    <m/>
+    <n v="2949.3"/>
+    <n v="15682.409999999993"/>
+    <x v="7"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-07T00:00:00"/>
+    <s v="CR"/>
+    <s v="SumUp Payments AccMDD PID748134"/>
+    <m/>
+    <n v="1327.17"/>
+    <n v="17009.579999999994"/>
+    <x v="7"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-08T00:00:00"/>
+    <s v="BP"/>
+    <s v="Vivian Shelton OAS"/>
+    <n v="112.87"/>
+    <m/>
+    <n v="16896.709999999995"/>
+    <x v="20"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Mrs C E Hopton OAS"/>
+    <n v="45"/>
+    <m/>
+    <n v="16851.709999999995"/>
+    <x v="14"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Miranda Miller OAS"/>
+    <n v="60"/>
+    <m/>
+    <n v="16791.709999999995"/>
+    <x v="14"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Anna Kolos OAS"/>
+    <n v="262.5"/>
+    <m/>
+    <n v="16529.209999999995"/>
+    <x v="14"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Peter Collins OAS"/>
+    <n v="67.5"/>
+    <m/>
+    <n v="16461.709999999995"/>
+    <x v="14"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Melinda Kenneway OAS"/>
+    <n v="896.25"/>
+    <m/>
+    <n v="15565.459999999995"/>
+    <x v="14"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Claire Drinkwater OAS"/>
+    <n v="93.75"/>
+    <m/>
+    <n v="15471.709999999995"/>
+    <x v="14"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="John Day OAS"/>
+    <n v="108.75"/>
+    <m/>
+    <n v="15362.959999999995"/>
+    <x v="14"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Hannah Farncombe OAS"/>
+    <n v="168.75"/>
+    <m/>
+    <n v="15194.209999999995"/>
+    <x v="14"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Harriet Calfo OAS"/>
+    <n v="262.5"/>
+    <m/>
+    <n v="14931.709999999995"/>
+    <x v="14"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="June Dent OAS"/>
+    <n v="221.25"/>
+    <m/>
+    <n v="14710.459999999995"/>
+    <x v="14"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Gerry Coles PrintsOAS"/>
+    <n v="48.75"/>
+    <m/>
+    <n v="14661.709999999995"/>
+    <x v="14"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Eirian Griffiths OAS"/>
+    <n v="172.5"/>
+    <m/>
+    <n v="14489.209999999995"/>
+    <x v="14"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Rod Craig OAS"/>
+    <n v="671.25"/>
+    <m/>
+    <n v="13817.959999999995"/>
+    <x v="14"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-10T00:00:00"/>
+    <s v="BP"/>
+    <s v="Tereza Horacek OAS"/>
+    <n v="187.5"/>
+    <m/>
+    <n v="13630.459999999995"/>
+    <x v="14"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-10T00:00:00"/>
+    <s v="BP"/>
+    <s v="Lizzie Wheeler OAS"/>
+    <n v="240"/>
+    <m/>
+    <n v="13390.459999999995"/>
+    <x v="14"/>
+    <s v="Open"/>
+  </r>
+  <r>
+    <d v="2024-10-10T00:00:00"/>
+    <s v="CR"/>
+    <s v="Stripe Payments UKSTRIPE"/>
+    <m/>
+    <n v="29.2"/>
+    <n v="13419.659999999996"/>
+    <x v="0"/>
+    <m/>
   </r>
   <r>
     <m/>
@@ -15865,71 +16344,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A5C2633A-7AD5-4920-9B01-65373321B481}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="E4:G8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField numFmtId="15" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="7"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Income" fld="4" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Expenditure" fld="3" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BE04C0F0-9A61-4F80-8276-3D04382D746D}" name="PivotTable2" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C28" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
@@ -15943,27 +16357,27 @@
       <items count="25">
         <item x="1"/>
         <item x="4"/>
+        <item x="8"/>
+        <item x="13"/>
+        <item x="12"/>
         <item x="7"/>
-        <item x="12"/>
-        <item x="11"/>
-        <item x="6"/>
-        <item x="13"/>
+        <item x="14"/>
         <item x="0"/>
         <item x="3"/>
-        <item x="15"/>
+        <item x="16"/>
         <item x="23"/>
         <item x="2"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="15"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="17"/>
+        <item x="5"/>
+        <item x="20"/>
         <item x="9"/>
-        <item x="10"/>
-        <item x="14"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="16"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="8"/>
         <item x="21"/>
-        <item x="5"/>
+        <item x="6"/>
         <item x="22"/>
         <item t="default"/>
       </items>
@@ -16077,6 +16491,71 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A5C2633A-7AD5-4920-9B01-65373321B481}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E4:G8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField numFmtId="15" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Income" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Expenditure" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{88CC6FF2-D2D5-4EC7-9086-AAE36B3B0E13}" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
@@ -16090,28 +16569,28 @@
     <pivotField axis="axisRow" showAll="0">
       <items count="25">
         <item x="1"/>
+        <item x="15"/>
+        <item x="4"/>
+        <item x="16"/>
+        <item x="11"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="8"/>
+        <item x="13"/>
+        <item x="10"/>
+        <item x="12"/>
+        <item x="7"/>
         <item x="14"/>
-        <item x="4"/>
-        <item x="15"/>
-        <item x="10"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="12"/>
-        <item x="9"/>
-        <item x="11"/>
-        <item x="6"/>
-        <item x="13"/>
         <item x="2"/>
         <item x="0"/>
         <item x="3"/>
-        <item x="16"/>
+        <item x="17"/>
         <item x="23"/>
-        <item x="19"/>
+        <item x="5"/>
         <item x="20"/>
-        <item x="8"/>
+        <item x="9"/>
         <item x="21"/>
-        <item x="5"/>
+        <item x="6"/>
         <item x="22"/>
         <item t="default"/>
       </items>
@@ -16196,7 +16675,7 @@
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2FE7C9AF-75EF-4873-8F1B-0F70A39EEC38}" name="PivotTable5" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A19:C27" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <location ref="A19:C28" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="15" showAll="0"/>
     <pivotField showAll="0"/>
@@ -16207,28 +16686,28 @@
     <pivotField axis="axisRow" showAll="0">
       <items count="25">
         <item x="1"/>
+        <item x="15"/>
+        <item x="4"/>
+        <item x="16"/>
+        <item x="11"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="8"/>
+        <item x="13"/>
+        <item x="10"/>
+        <item x="12"/>
+        <item x="7"/>
         <item x="14"/>
-        <item x="4"/>
-        <item x="15"/>
-        <item x="10"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="12"/>
-        <item x="9"/>
-        <item x="11"/>
-        <item x="6"/>
-        <item x="13"/>
         <item x="2"/>
         <item x="0"/>
         <item x="3"/>
-        <item x="16"/>
+        <item x="17"/>
         <item x="23"/>
-        <item x="19"/>
+        <item x="5"/>
         <item x="20"/>
-        <item x="8"/>
+        <item x="9"/>
         <item x="21"/>
-        <item x="5"/>
+        <item x="6"/>
         <item x="22"/>
         <item t="default"/>
       </items>
@@ -16246,7 +16725,7 @@
   <rowFields count="1">
     <field x="6"/>
   </rowFields>
-  <rowItems count="8">
+  <rowItems count="9">
     <i>
       <x v="7"/>
     </i>
@@ -16258,6 +16737,9 @@
     </i>
     <i>
       <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
     </i>
     <i>
       <x v="13"/>
@@ -16607,18 +17089,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="14.1796875" style="5" customWidth="1"/>
     <col min="3" max="4" width="8.1796875" style="5"/>
     <col min="5" max="5" width="16.54296875" style="5" customWidth="1"/>
     <col min="6" max="8" width="8.1796875" style="5"/>
     <col min="9" max="9" width="24.81640625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="11.36328125" style="5" customWidth="1"/>
     <col min="11" max="12" width="8.1796875" style="5"/>
-    <col min="13" max="13" width="22.453125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="22.36328125" style="5" customWidth="1"/>
     <col min="14" max="18" width="8.1796875" style="5"/>
     <col min="19" max="19" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.6328125" style="5" customWidth="1"/>
+    <col min="20" max="20" width="9.54296875" style="5" customWidth="1"/>
     <col min="21" max="16384" width="8.1796875" style="5"/>
   </cols>
   <sheetData>
@@ -17666,10 +18148,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60FA1291-B9CE-4F7D-8600-2336ADED0E75}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -17903,46 +18385,55 @@
         <v>808</v>
       </c>
       <c r="B23" s="40">
-        <v>3708.27</v>
+        <v>8864.61</v>
       </c>
       <c r="C23" s="40"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="40">
-        <v>8007.4999999999991</v>
-      </c>
-      <c r="C24" s="40"/>
+        <v>809</v>
+      </c>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40">
+        <v>3506.25</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="34" t="s">
-        <v>811</v>
-      </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40">
-        <v>231</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B25" s="40">
+        <v>8007.4999999999991</v>
+      </c>
+      <c r="C25" s="40"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="34" t="s">
-        <v>2207</v>
-      </c>
-      <c r="B26" s="40">
-        <v>116.57</v>
-      </c>
-      <c r="C26" s="40"/>
+        <v>811</v>
+      </c>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40">
+        <v>343.87</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="34" t="s">
+        <v>2207</v>
+      </c>
+      <c r="B27" s="40">
+        <v>116.57</v>
+      </c>
+      <c r="C27" s="40"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="34" t="s">
         <v>573</v>
       </c>
-      <c r="B27" s="40">
-        <v>11832.339999999998</v>
-      </c>
-      <c r="C27" s="40">
-        <v>780</v>
+      <c r="B28" s="40">
+        <v>16988.68</v>
+      </c>
+      <c r="C28" s="40">
+        <v>4399.12</v>
       </c>
     </row>
   </sheetData>
@@ -17952,10 +18443,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5956F534-76F9-4C2C-AE0C-5DBCF3D7B234}">
-  <dimension ref="A1:I320"/>
+  <dimension ref="A1:I340"/>
   <sheetViews>
-    <sheetView topLeftCell="A296" workbookViewId="0">
-      <selection activeCell="I319" sqref="I319"/>
+    <sheetView topLeftCell="A317" workbookViewId="0">
+      <selection activeCell="H340" sqref="H340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -22390,7 +22881,7 @@
         <v>14627.1</v>
       </c>
       <c r="G208" t="s">
-        <v>812</v>
+        <v>929</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
@@ -23610,7 +24101,7 @@
         <v>18</v>
       </c>
       <c r="F261" s="32">
-        <f t="shared" ref="F261:F320" si="4">F260+E261-D261</f>
+        <f t="shared" ref="F261:F325" si="4">F260+E261-D261</f>
         <v>8348.1099999999951</v>
       </c>
       <c r="G261" t="s">
@@ -25018,8 +25509,485 @@
         <v>870</v>
       </c>
     </row>
+    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A321" s="31">
+        <v>45568</v>
+      </c>
+      <c r="B321" t="s">
+        <v>396</v>
+      </c>
+      <c r="C321" t="s">
+        <v>2235</v>
+      </c>
+      <c r="E321">
+        <v>879.87</v>
+      </c>
+      <c r="F321" s="32">
+        <f t="shared" si="4"/>
+        <v>12733.109999999993</v>
+      </c>
+      <c r="G321" t="s">
+        <v>808</v>
+      </c>
+      <c r="H321" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A322" s="31">
+        <v>45569</v>
+      </c>
+      <c r="B322" t="s">
+        <v>396</v>
+      </c>
+      <c r="C322" t="s">
+        <v>2236</v>
+      </c>
+      <c r="E322">
+        <v>2949.3</v>
+      </c>
+      <c r="F322" s="32">
+        <f t="shared" si="4"/>
+        <v>15682.409999999993</v>
+      </c>
+      <c r="G322" t="s">
+        <v>808</v>
+      </c>
+      <c r="H322" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A323" s="31">
+        <v>45572</v>
+      </c>
+      <c r="B323" t="s">
+        <v>396</v>
+      </c>
+      <c r="C323" t="s">
+        <v>2237</v>
+      </c>
+      <c r="E323">
+        <v>1327.17</v>
+      </c>
+      <c r="F323" s="32">
+        <f t="shared" si="4"/>
+        <v>17009.579999999994</v>
+      </c>
+      <c r="G323" t="s">
+        <v>808</v>
+      </c>
+      <c r="H323" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A324" s="31">
+        <v>45573</v>
+      </c>
+      <c r="B324" t="s">
+        <v>541</v>
+      </c>
+      <c r="C324" t="s">
+        <v>2238</v>
+      </c>
+      <c r="D324">
+        <v>112.87</v>
+      </c>
+      <c r="F324" s="32">
+        <f t="shared" si="4"/>
+        <v>16896.709999999995</v>
+      </c>
+      <c r="G324" t="s">
+        <v>811</v>
+      </c>
+      <c r="H324" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A325" s="31">
+        <v>45574</v>
+      </c>
+      <c r="B325" t="s">
+        <v>541</v>
+      </c>
+      <c r="C325" t="s">
+        <v>2239</v>
+      </c>
+      <c r="D325">
+        <v>45</v>
+      </c>
+      <c r="F325" s="32">
+        <f t="shared" si="4"/>
+        <v>16851.709999999995</v>
+      </c>
+      <c r="G325" t="s">
+        <v>809</v>
+      </c>
+      <c r="H325" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A326" s="31">
+        <v>45574</v>
+      </c>
+      <c r="B326" t="s">
+        <v>541</v>
+      </c>
+      <c r="C326" t="s">
+        <v>2240</v>
+      </c>
+      <c r="D326">
+        <v>60</v>
+      </c>
+      <c r="F326" s="32">
+        <f t="shared" ref="F326:F340" si="5">F325+E326-D326</f>
+        <v>16791.709999999995</v>
+      </c>
+      <c r="G326" t="s">
+        <v>809</v>
+      </c>
+      <c r="H326" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A327" s="31">
+        <v>45574</v>
+      </c>
+      <c r="B327" t="s">
+        <v>541</v>
+      </c>
+      <c r="C327" t="s">
+        <v>2241</v>
+      </c>
+      <c r="D327">
+        <v>262.5</v>
+      </c>
+      <c r="F327" s="32">
+        <f t="shared" si="5"/>
+        <v>16529.209999999995</v>
+      </c>
+      <c r="G327" t="s">
+        <v>809</v>
+      </c>
+      <c r="H327" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A328" s="31">
+        <v>45574</v>
+      </c>
+      <c r="B328" t="s">
+        <v>541</v>
+      </c>
+      <c r="C328" t="s">
+        <v>2242</v>
+      </c>
+      <c r="D328">
+        <v>67.5</v>
+      </c>
+      <c r="F328" s="32">
+        <f t="shared" si="5"/>
+        <v>16461.709999999995</v>
+      </c>
+      <c r="G328" t="s">
+        <v>809</v>
+      </c>
+      <c r="H328" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A329" s="31">
+        <v>45574</v>
+      </c>
+      <c r="B329" t="s">
+        <v>541</v>
+      </c>
+      <c r="C329" t="s">
+        <v>2243</v>
+      </c>
+      <c r="D329">
+        <v>896.25</v>
+      </c>
+      <c r="F329" s="32">
+        <f t="shared" si="5"/>
+        <v>15565.459999999995</v>
+      </c>
+      <c r="G329" t="s">
+        <v>809</v>
+      </c>
+      <c r="H329" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A330" s="31">
+        <v>45574</v>
+      </c>
+      <c r="B330" t="s">
+        <v>541</v>
+      </c>
+      <c r="C330" t="s">
+        <v>2244</v>
+      </c>
+      <c r="D330">
+        <v>93.75</v>
+      </c>
+      <c r="F330" s="32">
+        <f t="shared" si="5"/>
+        <v>15471.709999999995</v>
+      </c>
+      <c r="G330" t="s">
+        <v>809</v>
+      </c>
+      <c r="H330" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A331" s="31">
+        <v>45574</v>
+      </c>
+      <c r="B331" t="s">
+        <v>541</v>
+      </c>
+      <c r="C331" t="s">
+        <v>2245</v>
+      </c>
+      <c r="D331">
+        <v>108.75</v>
+      </c>
+      <c r="F331" s="32">
+        <f t="shared" si="5"/>
+        <v>15362.959999999995</v>
+      </c>
+      <c r="G331" t="s">
+        <v>809</v>
+      </c>
+      <c r="H331" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A332" s="31">
+        <v>45574</v>
+      </c>
+      <c r="B332" t="s">
+        <v>541</v>
+      </c>
+      <c r="C332" t="s">
+        <v>2246</v>
+      </c>
+      <c r="D332">
+        <v>168.75</v>
+      </c>
+      <c r="F332" s="32">
+        <f t="shared" si="5"/>
+        <v>15194.209999999995</v>
+      </c>
+      <c r="G332" t="s">
+        <v>809</v>
+      </c>
+      <c r="H332" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A333" s="31">
+        <v>45574</v>
+      </c>
+      <c r="B333" t="s">
+        <v>541</v>
+      </c>
+      <c r="C333" t="s">
+        <v>2247</v>
+      </c>
+      <c r="D333">
+        <v>262.5</v>
+      </c>
+      <c r="F333" s="32">
+        <f t="shared" si="5"/>
+        <v>14931.709999999995</v>
+      </c>
+      <c r="G333" t="s">
+        <v>809</v>
+      </c>
+      <c r="H333" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A334" s="31">
+        <v>45574</v>
+      </c>
+      <c r="B334" t="s">
+        <v>541</v>
+      </c>
+      <c r="C334" t="s">
+        <v>2248</v>
+      </c>
+      <c r="D334">
+        <v>221.25</v>
+      </c>
+      <c r="F334" s="32">
+        <f t="shared" si="5"/>
+        <v>14710.459999999995</v>
+      </c>
+      <c r="G334" t="s">
+        <v>809</v>
+      </c>
+      <c r="H334" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A335" s="31">
+        <v>45574</v>
+      </c>
+      <c r="B335" t="s">
+        <v>541</v>
+      </c>
+      <c r="C335" t="s">
+        <v>2249</v>
+      </c>
+      <c r="D335">
+        <v>48.75</v>
+      </c>
+      <c r="F335" s="32">
+        <f t="shared" si="5"/>
+        <v>14661.709999999995</v>
+      </c>
+      <c r="G335" t="s">
+        <v>809</v>
+      </c>
+      <c r="H335" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A336" s="31">
+        <v>45574</v>
+      </c>
+      <c r="B336" t="s">
+        <v>541</v>
+      </c>
+      <c r="C336" t="s">
+        <v>2250</v>
+      </c>
+      <c r="D336">
+        <v>172.5</v>
+      </c>
+      <c r="F336" s="32">
+        <f t="shared" si="5"/>
+        <v>14489.209999999995</v>
+      </c>
+      <c r="G336" t="s">
+        <v>809</v>
+      </c>
+      <c r="H336" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A337" s="31">
+        <v>45574</v>
+      </c>
+      <c r="B337" t="s">
+        <v>541</v>
+      </c>
+      <c r="C337" t="s">
+        <v>2251</v>
+      </c>
+      <c r="D337">
+        <v>671.25</v>
+      </c>
+      <c r="F337" s="32">
+        <f t="shared" si="5"/>
+        <v>13817.959999999995</v>
+      </c>
+      <c r="G337" t="s">
+        <v>809</v>
+      </c>
+      <c r="H337" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A338" s="31">
+        <v>45575</v>
+      </c>
+      <c r="B338" t="s">
+        <v>541</v>
+      </c>
+      <c r="C338" t="s">
+        <v>2252</v>
+      </c>
+      <c r="D338">
+        <v>187.5</v>
+      </c>
+      <c r="F338" s="32">
+        <f t="shared" si="5"/>
+        <v>13630.459999999995</v>
+      </c>
+      <c r="G338" t="s">
+        <v>809</v>
+      </c>
+      <c r="H338" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A339" s="31">
+        <v>45575</v>
+      </c>
+      <c r="B339" t="s">
+        <v>541</v>
+      </c>
+      <c r="C339" t="s">
+        <v>2253</v>
+      </c>
+      <c r="D339">
+        <v>240</v>
+      </c>
+      <c r="F339" s="32">
+        <f t="shared" si="5"/>
+        <v>13390.459999999995</v>
+      </c>
+      <c r="G339" t="s">
+        <v>809</v>
+      </c>
+      <c r="H339" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A340" s="31">
+        <v>45575</v>
+      </c>
+      <c r="B340" t="s">
+        <v>396</v>
+      </c>
+      <c r="C340" t="s">
+        <v>828</v>
+      </c>
+      <c r="E340">
+        <v>29.2</v>
+      </c>
+      <c r="F340" s="32">
+        <f t="shared" si="5"/>
+        <v>13419.659999999996</v>
+      </c>
+      <c r="G340" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I313" xr:uid="{5956F534-76F9-4C2C-AE0C-5DBCF3D7B234}"/>
+  <autoFilter ref="A1:I323" xr:uid="{5956F534-76F9-4C2C-AE0C-5DBCF3D7B234}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -43307,22 +44275,22 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="9" style="5"/>
-    <col min="3" max="3" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.1796875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="5"/>
-    <col min="7" max="7" width="10.453125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" style="5" customWidth="1"/>
     <col min="8" max="8" width="2.7265625" style="5" customWidth="1"/>
     <col min="9" max="9" width="9" style="5"/>
-    <col min="10" max="10" width="17.453125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="17.36328125" style="5" customWidth="1"/>
     <col min="11" max="11" width="35.1796875" style="5" customWidth="1"/>
     <col min="12" max="12" width="9" style="5" customWidth="1"/>
     <col min="13" max="13" width="22" style="5" customWidth="1"/>
     <col min="14" max="14" width="7.453125" style="5" customWidth="1"/>
     <col min="15" max="15" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.81640625" style="5" customWidth="1"/>
-    <col min="18" max="18" width="10.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
@@ -43992,25 +44960,25 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB58F2B2-604E-41D7-8D60-AEC068EC3CDA}">
-  <dimension ref="A1:AH20"/>
+  <dimension ref="A1:AH25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10:J13"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="9" style="5"/>
-    <col min="3" max="3" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.36328125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.81640625" style="5" customWidth="1"/>
     <col min="6" max="7" width="9" style="5"/>
-    <col min="8" max="8" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21" style="5" customWidth="1"/>
     <col min="10" max="10" width="13.90625" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="26" width="9" style="5"/>
     <col min="27" max="27" width="25.1796875" style="5" customWidth="1"/>
-    <col min="28" max="28" width="32.81640625" style="5" customWidth="1"/>
+    <col min="28" max="28" width="32.7265625" style="5" customWidth="1"/>
     <col min="29" max="29" width="9" style="9"/>
     <col min="30" max="30" width="9" style="5"/>
     <col min="31" max="32" width="15.54296875" style="5" customWidth="1"/>
@@ -44095,23 +45063,23 @@
         <v>60</v>
       </c>
       <c r="D3" s="35">
-        <f t="shared" ref="D3:D14" si="0">C3*0.25</f>
+        <f t="shared" ref="D3:D21" si="0">C3*0.25</f>
         <v>15</v>
       </c>
       <c r="E3" s="35">
-        <f t="shared" ref="E3:E14" si="1">C3-D3</f>
+        <f t="shared" ref="E3:E21" si="1">C3-D3</f>
         <v>45</v>
       </c>
       <c r="F3"/>
       <c r="G3" s="37">
-        <f t="shared" ref="G3:G14" si="2">0.0169*C3</f>
+        <f t="shared" ref="G3:G21" si="2">0.0169*C3</f>
         <v>1.0139999999999998</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>2224</v>
       </c>
       <c r="J3" s="37">
-        <f t="shared" ref="J3:J14" si="3">C3-G3</f>
+        <f t="shared" ref="J3:J21" si="3">C3-G3</f>
         <v>58.985999999999997</v>
       </c>
       <c r="AG3" s="2"/>
@@ -44424,59 +45392,230 @@
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="G15" s="37"/>
-      <c r="J15" s="37"/>
+      <c r="C15" s="35">
+        <v>895</v>
+      </c>
+      <c r="D15" s="35">
+        <f t="shared" si="0"/>
+        <v>223.75</v>
+      </c>
+      <c r="E15" s="35">
+        <f t="shared" si="1"/>
+        <v>671.25</v>
+      </c>
+      <c r="G15" s="37">
+        <f t="shared" si="2"/>
+        <v>15.125499999999999</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>2224</v>
+      </c>
+      <c r="J15" s="37">
+        <f t="shared" si="3"/>
+        <v>879.87450000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="C16" s="35">
+        <v>3000</v>
+      </c>
+      <c r="D16" s="35">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+      <c r="E16" s="35">
+        <f t="shared" si="1"/>
+        <v>2250</v>
+      </c>
+      <c r="G16" s="37">
+        <f t="shared" si="2"/>
+        <v>50.699999999999996</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>2224</v>
+      </c>
+      <c r="J16" s="37">
+        <f t="shared" si="3"/>
+        <v>2949.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C17" s="35">
+        <v>295</v>
+      </c>
+      <c r="D17" s="35">
+        <f t="shared" si="0"/>
+        <v>73.75</v>
+      </c>
+      <c r="E17" s="35">
+        <f t="shared" si="1"/>
+        <v>221.25</v>
+      </c>
+      <c r="G17" s="37">
+        <f t="shared" si="2"/>
+        <v>4.9854999999999992</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>2224</v>
+      </c>
+      <c r="J17" s="37">
+        <f t="shared" si="3"/>
+        <v>290.0145</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="C18" s="35">
+        <v>350</v>
+      </c>
+      <c r="D18" s="35">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="E18" s="35">
+        <f t="shared" si="1"/>
+        <v>262.5</v>
+      </c>
+      <c r="G18" s="37">
+        <f t="shared" si="2"/>
+        <v>5.9149999999999991</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>2224</v>
+      </c>
+      <c r="J18" s="37">
+        <f t="shared" si="3"/>
+        <v>344.08499999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C19" s="35">
+        <v>230</v>
+      </c>
+      <c r="D19" s="35">
+        <f t="shared" si="0"/>
+        <v>57.5</v>
+      </c>
+      <c r="E19" s="35">
+        <f t="shared" si="1"/>
+        <v>172.5</v>
+      </c>
+      <c r="G19" s="37">
+        <f t="shared" si="2"/>
+        <v>3.8869999999999996</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>2224</v>
+      </c>
+      <c r="J19" s="37">
+        <f t="shared" si="3"/>
+        <v>226.113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C20" s="35">
+        <v>200</v>
+      </c>
+      <c r="D20" s="35">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="E20" s="35">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="G20" s="37">
+        <f t="shared" si="2"/>
+        <v>3.38</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>2224</v>
+      </c>
+      <c r="J20" s="37">
+        <f t="shared" si="3"/>
+        <v>196.62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C21" s="35">
+        <v>275</v>
+      </c>
+      <c r="D21" s="35">
+        <f t="shared" si="0"/>
+        <v>68.75</v>
+      </c>
+      <c r="E21" s="35">
+        <f t="shared" si="1"/>
+        <v>206.25</v>
+      </c>
+      <c r="G21" s="37">
+        <f t="shared" si="2"/>
+        <v>4.6475</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>2224</v>
+      </c>
+      <c r="J21" s="37">
+        <f t="shared" si="3"/>
+        <v>270.35250000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="G22" s="37"/>
+      <c r="J22" s="37"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>2220</v>
       </c>
-      <c r="C18" s="37">
-        <f>SUM(C2:C17)</f>
-        <v>3770</v>
-      </c>
-      <c r="D18" s="37">
-        <f t="shared" ref="D18:E18" si="4">SUM(D2:D17)</f>
-        <v>942.5</v>
-      </c>
-      <c r="E18" s="37">
+      <c r="C23" s="37">
+        <f>SUM(C2:C21)</f>
+        <v>9015</v>
+      </c>
+      <c r="D23" s="37">
+        <f t="shared" ref="D23:E23" si="4">SUM(D2:D21)</f>
+        <v>2253.75</v>
+      </c>
+      <c r="E23" s="37">
         <f t="shared" si="4"/>
-        <v>2827.5</v>
-      </c>
-      <c r="G18" s="37">
-        <f>SUM(G2:G17)</f>
-        <v>61.727000000000004</v>
-      </c>
-      <c r="J18" s="37">
-        <f>SUM(J2:J17)</f>
-        <v>3708.2729999999992</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+        <v>6761.25</v>
+      </c>
+      <c r="G23" s="37">
+        <f>SUM(G2:G21)</f>
+        <v>150.36750000000001</v>
+      </c>
+      <c r="J23" s="37">
+        <f>SUM(J2:J21)</f>
+        <v>8864.6325000000015</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
         <v>2221</v>
       </c>
-      <c r="C19" s="5">
-        <f>COUNT(C2:C17)</f>
-        <v>13</v>
-      </c>
-      <c r="I19" s="5" t="s">
+      <c r="C24" s="5">
+        <f>COUNT(C2:C21)+1</f>
+        <v>21</v>
+      </c>
+      <c r="I24" s="5" t="s">
         <v>2228</v>
       </c>
-      <c r="J19" s="37">
-        <f>E18</f>
-        <v>2827.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J20" s="39">
-        <f>J18-J19</f>
-        <v>880.77299999999923</v>
+      <c r="J24" s="37">
+        <f>E23</f>
+        <v>6761.25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J25" s="39">
+        <f>J23-J24</f>
+        <v>2103.3825000000015</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:X274">
-    <sortCondition ref="E3:E274"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:X279">
+    <sortCondition ref="E3:E279"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -44667,10 +45806,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" customWidth="1"/>
+    <col min="1" max="1" width="11.36328125" customWidth="1"/>
     <col min="2" max="2" width="18.6328125" customWidth="1"/>
     <col min="3" max="3" width="18.1796875" customWidth="1"/>
-    <col min="4" max="20" width="12.7265625" style="2" customWidth="1"/>
+    <col min="4" max="20" width="12.6328125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="13.5" x14ac:dyDescent="0.3">
@@ -45866,11 +47005,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" style="5" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6328125" style="5" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="16.7265625" style="5" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" style="5" customWidth="1"/>
     <col min="4" max="5" width="8.1796875" style="5"/>
-    <col min="6" max="6" width="11" style="5" customWidth="1"/>
+    <col min="6" max="6" width="11.08984375" style="5" customWidth="1"/>
     <col min="7" max="7" width="8.1796875" style="5"/>
     <col min="8" max="8" width="10.6328125" style="5" customWidth="1"/>
     <col min="9" max="9" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
@@ -46041,14 +47180,14 @@
     <col min="1" max="2" width="9" style="5"/>
     <col min="3" max="3" width="15.26953125" style="5" customWidth="1"/>
     <col min="4" max="14" width="9" style="5"/>
-    <col min="15" max="16" width="18.81640625" style="5" customWidth="1"/>
+    <col min="15" max="16" width="18.90625" style="5" customWidth="1"/>
     <col min="17" max="19" width="9" style="5"/>
     <col min="20" max="21" width="32.1796875" style="5" customWidth="1"/>
     <col min="22" max="22" width="18.453125" style="5" customWidth="1"/>
     <col min="23" max="23" width="9" style="5"/>
-    <col min="24" max="24" width="11" style="5" customWidth="1"/>
+    <col min="24" max="24" width="11.08984375" style="5" customWidth="1"/>
     <col min="25" max="25" width="9" style="5"/>
-    <col min="26" max="26" width="10.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14.453125" style="5" customWidth="1"/>
     <col min="28" max="16384" width="9" style="5"/>
   </cols>
@@ -48939,7 +50078,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
@@ -49016,7 +50155,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -49286,7 +50425,7 @@
   <dimension ref="A3:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -49294,11 +50433,11 @@
     <col min="1" max="1" width="21.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="18" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="18" width="23.6328125" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="11.08984375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="13.36328125" bestFit="1" customWidth="1"/>
@@ -49309,7 +50448,7 @@
     <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="15" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.6328125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="15" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="15" bestFit="1" customWidth="1"/>
@@ -49319,11 +50458,11 @@
     <col min="37" max="37" width="15" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="20" bestFit="1" customWidth="1"/>
-    <col min="40" max="41" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="6.90625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="45" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="45" width="6.90625" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="49" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="49" width="6.90625" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="6.7265625" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="11.08984375" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="15" bestFit="1" customWidth="1"/>
@@ -49403,7 +50542,7 @@
     <col min="126" max="126" width="15" bestFit="1" customWidth="1"/>
     <col min="127" max="127" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="128" max="128" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="130" max="130" width="15" bestFit="1" customWidth="1"/>
     <col min="131" max="131" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="132" max="132" width="21.26953125" bestFit="1" customWidth="1"/>
@@ -49439,7 +50578,7 @@
     <col min="162" max="162" width="15" bestFit="1" customWidth="1"/>
     <col min="163" max="163" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="164" max="164" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="165" max="165" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="165" max="165" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="166" max="166" width="15" bestFit="1" customWidth="1"/>
     <col min="167" max="167" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="168" max="168" width="21.26953125" bestFit="1" customWidth="1"/>
@@ -49455,7 +50594,7 @@
     <col min="178" max="178" width="15" bestFit="1" customWidth="1"/>
     <col min="179" max="179" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="180" max="180" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="181" max="181" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="181" max="181" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="182" max="182" width="15" bestFit="1" customWidth="1"/>
     <col min="183" max="183" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="184" max="184" width="21.26953125" bestFit="1" customWidth="1"/>
@@ -49504,9 +50643,8 @@
     <col min="227" max="227" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="228" max="228" width="15" bestFit="1" customWidth="1"/>
     <col min="229" max="229" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="230" max="230" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="231" max="231" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="232" max="232" width="20" bestFit="1" customWidth="1"/>
+    <col min="230" max="230" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="231" max="232" width="20" bestFit="1" customWidth="1"/>
     <col min="233" max="233" width="18.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -49544,7 +50682,7 @@
         <v>812</v>
       </c>
       <c r="B5" s="40">
-        <v>100.98</v>
+        <v>100</v>
       </c>
       <c r="C5" s="40"/>
       <c r="E5" s="34" t="s">
@@ -49569,10 +50707,10 @@
         <v>870</v>
       </c>
       <c r="F6" s="40">
-        <v>11832.340000000002</v>
+        <v>16988.68</v>
       </c>
       <c r="G6" s="40">
-        <v>780</v>
+        <v>4399.12</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -49587,7 +50725,7 @@
         <v>574</v>
       </c>
       <c r="F7" s="40">
-        <v>7449.9100000000008</v>
+        <v>7479.1100000000006</v>
       </c>
       <c r="G7" s="40">
         <v>11467.09</v>
@@ -49605,10 +50743,10 @@
         <v>573</v>
       </c>
       <c r="F8" s="40">
-        <v>25789.9</v>
+        <v>30975.440000000002</v>
       </c>
       <c r="G8" s="40">
-        <v>18966.27</v>
+        <v>22585.39</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -49616,7 +50754,7 @@
         <v>808</v>
       </c>
       <c r="B9" s="40">
-        <v>7331.95</v>
+        <v>12488.289999999999</v>
       </c>
       <c r="C9" s="40"/>
     </row>
@@ -49626,7 +50764,7 @@
       </c>
       <c r="B10" s="40"/>
       <c r="C10" s="40">
-        <v>2632.5</v>
+        <v>6138.75</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -49634,7 +50772,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="40">
-        <v>7447.9500000000016</v>
+        <v>7477.1500000000015</v>
       </c>
       <c r="C11" s="40"/>
     </row>
@@ -49731,7 +50869,7 @@
         <v>929</v>
       </c>
       <c r="B22" s="40">
-        <v>0.98</v>
+        <v>1.96</v>
       </c>
       <c r="C22" s="40"/>
     </row>
@@ -49741,7 +50879,7 @@
       </c>
       <c r="B23" s="40"/>
       <c r="C23" s="40">
-        <v>231</v>
+        <v>343.87</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -49785,10 +50923,10 @@
         <v>573</v>
       </c>
       <c r="B28" s="40">
-        <v>25789.9</v>
+        <v>30975.440000000002</v>
       </c>
       <c r="C28" s="40">
-        <v>18966.270000000004</v>
+        <v>22585.390000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>